<commit_message>
Added new regional 2012 assessments file
</commit_message>
<xml_diff>
--- a/src/wise/msfd/data/Regional_Descriptors_2012_assessment.xlsx
+++ b/src/wise/msfd/data/Regional_Descriptors_2012_assessment.xlsx
@@ -8,8 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Instructions" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Assessment" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Conclusions" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Instructions" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="295">
   <si>
     <t xml:space="preserve">Region</t>
   </si>
@@ -445,7 +446,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
+    <t xml:space="preserve">n/a</t>
   </si>
   <si>
     <t xml:space="preserve">D11</t>
@@ -493,6 +494,961 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">NEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The level of coherence across the North East Atlantic marine region for the definition of Good Environmental Status for Descriptor 1 is low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All ten Member States of the marine region have defined GES for Descriptor 1 but none have defined it in the same way (or even similarly). The levels of details vary enormously. This being said, all Member States but one (NL) have defined GES more specifically than in the text of Annex I of the MSFD and most Member States have incorporated some or all of the Commission Decision criteria for D1. Five Member States have provided specific definitions for each criterion (BE partially, DK, ES, FR, SE) and three Member States have covered certain criteria but not all (IE, PT, UK). Only two Member States do not cover the Commission Decision criteria at all (DE, NL). The coverage of the Commission Decision indicators is much less systematic with only two Member States covering all or most indicators but without necessarily all elements to make them measurable (ES, FR) and other Member States covering them only partially (DK, IE, SE, UK). 
+For a majority of Member States, the GES definition covers at least the species, habitats and ecosystem levels (BE, DK, ES, IE, FR, PT, SE, UK) but to varying levels of details. 
+With regard to the definition at species level, half of the Member States address the three main highly-mobile species groups –mammals, birds and fish (BE, DK, NL, SE, UK). For four Member States, specific species groups are not explicitly mentioned (DE, FR, IE, PT). The concept of species groups is what is mostly used by Member States. Only two Member States use the concept of functional groups, in addition to species groups (ES, FR). Out of these two, only one Member State covers cephalopods and reptiles in its GES definition (ES). Two Member States have included shellfish in the scope of their GES definition (DK, ES). 
+In terms of individual species addressed in the GES definitions, three different approaches are apparent. For two Member States, the GES definition addresses all species and individual species are not singled out (NL, PT). For others, individual species are mentioned (as indicators) but it is still clear from the GES definition that all species are covered (BE, FR, UK). Finally, for a third group of Member States, it is not clear whether all species are covered by the GES definition or only the ones explicitly mentioned in the definition (DK, ES, IE, SE). For one Member State, only protected/listed species are addressed by the definition (DE). When individual species are referred to, a number of them are most commonly used as indicators for the GES definitions. In particular for mammals, the use of the harbour porpoise, the seal (several species of seals) and to a more limited extent certain whales and dolphins is relatively common (five Member States out of ten). Some Member States have referred to types of species (e.g. long-lived slowly reproducing species, top predators) (e.g. BE, DK).
+Only half of the Member States have included a specific mention to listed/protected species in their GES definitions (BE, DE, ES only to a limited extent, IE, UK). These include species covered by the Habitats and Birds Directives and species protected by the OSPAR Convention, the IUCN list of endangered species and the ASCOBANS and ACCOBAMS Agreements. 
+The level of coherence of the Member States’ reporting at the species level is moderate.
+With regard to the definitions at habitats level, the habitat types/zones covered by the GES definitions of the countries of the North East Atlantic marine region are defined in very different ways. Only one Member State uses the concept of predominant habitats as defined for the purpose of the MSFD and not even directly in its definition but in its accompanying text (FR). One Member State (DK) refers to the concept of predominant habitats but without actually specifying the predominant habitat types covered by its definition (except for a distinction between hard and soft bottoms). Six Member States out of ten are not specific with regard to the habitat types covered by their GES definition (BE, DE, ES, IE, NL, PT) but for two out of these six Member States, it seems that in any case only seabed habitats are covered (ES, NL). For the other Member States, the lack of specificity seems to indicate that all habitats are covered by the GES definition, except for one Member State (DE), which clearly covers only protected/listed habitats. One Member State mentions hard-bottom habitats and soft-bottom habitats as the two main habitat types covered by its GES (DK). Only two Member States provide a detailed list of the habitats covered in their GES definition, covering both benthic and pelagic habitats (SE, UK). Only few Member States have covered all the main relevant zones for seabed habitats (intertidal, shallow, shelf, bathyal/abyssal). Two Member States specifically mention the use of the (coarse) EUNIS level 2 habitat classification (SE, UK). 
+Only half of the Member States in the marine region have included a specific mention to listed/protected habitats in their GES definitions (BE, DE, ES, IE, UK). These include mainly habitats from the Habitats Directives and protected by the OSPAR Convention. 
+The level of coherence of the Member States’ reporting at the habitats level is much lower than at species level.
+With regard to the definitions at ecosystem level, a majority of Member States have defined GES so that it covers the whole ecosystem structure (DK, ES, FR, IE, PT, SE – but less clearly, UK). In addition, two of these Member States have set specific indicators for criterion 1.7 but only based on the condition of the birds and fish communities (ES, SE). 
+Most of the GES definitions for D1 in the North East Atlantic region are qualitative. Only a limited number of Member States have defined quantitative threshold values along with their GES definition and when they have done so, they have defined these only for specific species/habitats, using different thresholds for different features (ES, SE, UK through their targets). 
+In terms of baselines, the approaches adopted by the Member States again vary greatly. A majority of Member States however have used baselines in the sense of ‘reference conditions’, i.e. in relation to ‘prevailing physiographic, geographic and climatic (natural) conditions’ that are largely free from anthropogenic influences (ES, FR, IE, PT, SE, UK). Out of these, only three Member States have integrated the principle of ‘reference condition plus acceptable deviation’ (ES, FR, UK) and out of these, only two Member States (FR, UK) have acknowledged natural/climatic variations and ecosystem dynamics and have not sought a rigid state for particular biodiversity components. Finally, two Member States have included the notion of ‘restoration’ of biodiversity in their definitions (IE, UK). 
+Half of the Member States have reflected, directly or indirectly, the definitions for Favourable Conservation Status under the Habitats Directive and/or for Good Ecological Status under the Water Framework Directive (BE, DE, ES, SE, UK). In some cases, the reference is made at a general level (DE, BE), while in other cases the reference is made for specific ecosystem components (ES, SE, UK). One Member State (ES) has clearly stated that it will tend towards achieving FCS for all ecosystem features however its achievement is not considered realistic in the timeframe of the MSFD. 
+Finally, all but one Member State (DK) have included in their GES definitions a reference to relevant regional and international agreements: OSPAR in general by seven Member States (BE, DE, ES, FR, IE, SE, UK) and OSPAR EcoQOs by three Member States (BE, DE, ES), ASCOBANS by five Member States (DE, ES, FR, SE, UK), HELCOM by two of the Member States with marine waters in the Baltic marine region (DE, SE) and the Convention on Biological Diversity (CBD) by only one Member State (PT).
+All ten Member States of the marine region have defined GES for Descriptor 1 but none have defined it in the same way (or even similarly). The levels of details vary enormously. This being said, all Member States but one (NL) have defined GES more specifically than in the text of Annex I of the MSFD and most Member States have incorporated some or all of the Commission Decision criteria for D1. Five Member States have provided specific definitions for each criterion (BE partially, DK, ES, FR, SE) and three Member States have covered certain criteria but not all (IE, PT, UK). Only two Member States do not cover the Commission Decision criteria at all (DE, NL). The coverage of the Commission Decision indicators is much less systematic with only two Member States covering all or most indicators but without necessarily all elements to make them measurable (ES, FR) and other Member States covering them only partially (DK, IE, SE, UK). 
+For a majority of Member States, the GES definition covers at least the species, habitats and ecosystem levels (BE, DK, ES, IE, FR, PT, SE, UK) but to varying levels of details. 
+With regard to the definition at species level, half of the Member States address the three main highly-mobile species groups –mammals, birds and fish (BE, DK, NL, SE, UK). For four Member States, specific species groups are not explicitly mentioned (DE, FR, IE, PT). The concept of species groups is what is mostly used by Member States. Only two Member States use the concept of functional groups, in addition to species groups (ES, FR). Out of these two, only one Member State covers cephalopods and reptiles in its GES definition (ES). Two Member States have included shellfish in the scope of their GES definition (DK, ES). 
+In terms of individual species addressed in the GES definitions, three different approaches are apparent. For two Member States, the GES definition addresses all species and individual species are not singled out (NL, PT). For others, individual species are mentioned (as indicators) but it is still clear from the GES definition that all species are covered (BE, FR, UK). Finally, for a third group of Member States, it is not clear whether all species are covered by the GES definition or only the ones explicitly mentioned in the definition (DK, ES, IE, SE). For one Member State, only protected/listed species are addressed by the definition (DE). When individual species are referred to, a number of them are most commonly used as indicators for the GES definitions. In particular for mammals, the use of the harbour porpoise, the seal (several species of seals) and to a more limited extent certain whales and dolphins is relatively common (five Member States out of ten). Some Member States have referred to types of species (e.g. long-lived slowly reproducing species, top predators) (e.g. BE, DK).
+Only half of the Member States have included a specific mention to listed/protected species in their GES definitions (BE, DE, ES only to a limited extent, IE, UK). These include species covered by the Habitats and Birds Directives and species protected by the OSPAR Convention, the IUCN list of endangered species and the ASCOBANS and ACCOBAMS Agreements. 
+The level of coherence of the Member States’ reporting at the species level is moderate.
+With regard to the definitions at habitats level, the habitat types/zones covered by the GES definitions of the countries of the North East Atlantic marine region are defined in very different ways. Only one Member State uses the concept of predominant habitats as defined for the purpose of the MSFD and not even directly in its definition but in its accompanying text (FR). One Member State (DK) refers to the concept of predominant habitats but without actually specifying the predominant habitat types covered by its definition (except for a distinction between hard and soft bottoms). Six Member States out of ten are not specific with regard to the habitat types covered by their GES definition (BE, DE, ES, IE, NL, PT) but for two out of these six Member States, it seems that in any case only seabed habitats are covered (ES, NL). For the other Member States, the lack of specificity seems to indicate that all habitats are covered by the GES definition, except for one Member State (DE), which clearly covers only protected/listed habitats. One Member State mentions hard-bottom habitats and soft-bottom habitats as the two main habitat types covered by its GES (DK). Only two Member States provide a detailed list of the habitats covered in their GES definition, covering both benthic and pelagic habitats (SE, UK). Only few Member States have covered all the main relevant zones for seabed habitats (intertidal, shallow, shelf, bathyal/abyssal). Two Member States specifically mention the use of the (coarse) EUNIS level 2 habitat classification (SE, UK). 
+Only half of the Member States in the marine region have included a specific mention to listed/protected habitats in their GES definitions (BE, DE, ES, IE, UK). These include mainly habitats from the Habitats Directives and protected by the OSPAR Convention. 
+The level of coherence of the Member States’ reporting at the habitats level is much lower than at species level.
+With regard to the definitions at ecosystem level, a majority of Member States have defined GES so that it covers the whole ecosystem structure (DK, ES, FR, IE, PT, SE – but less clearly, UK). In addition, two of these Member States have set specific indicators for criterion 1.7 but only based on the condition of the birds and fish communities (ES, SE). 
+Most of the GES definitions for D1 in the North East Atlantic region are qualitative. Only a limited number of Member States have defined quantitative threshold values along with their GES definition and when they have done so, they have defined these only for specific species/habitats, using different thresholds for different features (ES, SE, UK through their targets). 
+In terms of baselines, the approaches adopted by the Member States again vary greatly. A majority of Member States however have used baselines in the sense of ‘reference conditions’, i.e. in relation to ‘prevailing physiographic, geographic and climatic (natural) conditions’ that are largely free from anthropogenic influences (ES, FR, IE, PT, SE, UK). Out of these, only three Member States have integrated the principle of ‘reference condition plus acceptable deviation’ (ES, FR, UK) and out of these, only two Member States (FR, UK) have acknowledged natural/climatic variations and ecosystem dynamics and have not sought a rigid state for particular biodiversity components. Finally, two Member States have included the notion of ‘restoration’ of biodiversity in their definitions (IE, UK). 
+Half of the Member States have reflected, directly or indirectly, the definitions for Favourable Conservation Status under the Habitats Directive and/or for Good Ecological Status under the Water Framework Directive (BE, DE, ES, SE, UK). In some cases, the reference is made at a general level (DE, BE), while in other cases the reference is made for specific ecosystem components (ES, SE, UK). One Member State (ES) has clearly stated that it will tend towards achieving FCS for all ecosystem features however its achievement is not considered realistic in the timeframe of the MSFD. 
+Finally, all but one Member State (DK) have included in their GES definitions a reference to relevant regional and international agreements: OSPAR in general by seven Member States (BE, DE, ES, FR, IE, SE, UK) and OSPAR EcoQOs by three Member States (BE, DE, ES), ASCOBANS by five Member States (DE, ES, FR, SE, UK), HELCOM by two of the Member States with marine waters in the Baltic marine region (DE, SE) and the Convention on Biological Diversity (CBD) by only one Member State (PT).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The level of coherence of the initial assessments on physical damage and loss across the North East Atlantic marine region is relatively high. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have undertaken an initial assessment on physical loss and physical damage.
+All Member States have covered most types of physical loss and physical damage. Likewise, all Member States have covered the main causes of pressure albeit at different levels of detail. Thus, while two Member States (ES, PT) report comprehensively on each type of pressure, including quantifying some parameters, in other Member States (e.g. BE, UK) the information focuses only on certain types of pressures and is more limited. The impacts of physical loss and physical damage are also covered by all Member States although some have not covered them in much detail (DE, IE, NL, SE). 
+Member States refer expressly to WFD reports (e.g. BE and IE) or to OSPAR relevant documents (e.g. DK and IE). Only one Member State (DK) presented clear conclusive judgements on the level of pressure of physical loss and physical damage and their impacts.
+In the reporting sheets, half of the Member States (BE, DK, ES, IE, NL) report that less than 1% of their assessment area (and of their seabed habitats) is affected by physical loss. The other Member States (DE, FR, SE, UK) do not report anything. For physical damage, there is more variation as one Member State (ES) reports that less than 1% of its assessment area is affected, two Member States (IE, UK) report 5-25%, one Member State (SE) reports 50-75% and three Member States (BE, DK, NL) report that 75 to 100% of their assessment area (and seabed habitats) is affected. The other Member States (DE, FR) do not report anything
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have undertaken an initial assessment on biological features. All Member States have reported on habitats and species/functional groups, but only a minority addressed ecosystems (DK, ES, NL). The level of coherence of the initial assessments on biological features across the North East Atlantic marine region is considered as low. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitats
+While most Member States covered at least a good share of the relevant seabed habitat types, more than half of Member States did not cover, or covered in a very limited way, water column habitat types (BE, DE, DK, ES, IE and NL). The majority of Member States used the MSFD classification of predominant habitats or an equivalent system (in particular EUNIS Level 2 classification), although in some cases the correspondence is not entirely clear (e.g. BE). When assessing habitats, all Member States reported on habitat distribution, extent and condition, as well as on the main causes of pressure (albeit with different levels of detail). However, only three Member States (PT, SE, UK) have provided a clear and conclusive judgement on the current status of the habitats. The Habitats Directive is mentioned by nine out of ten Member States (except DE and the North Sea subregion in FR) as are OSPAR and other relevant international conventions.
+In the reporting sheets, three Member States (BE, DK, ES) reported on listed habitats from the Habitats Directive, despite agreement that this reporting should be deferred to the 2013 reporting processes under these two Directives, and four Member States (DE, DK, ES, IE) reported on listed habitats from the OSPAR Convention. All Member States that have reported (i.e. all Member States from the region minus Portugal) have reported using the MSFD predominant habitat type classification. The predominant habitat types which have been most reported are shallow sand (6 Member States), shelf coarse sediment (6 Member States), shelf mixed sediment (6 Member States) and shallow mud (5 Member States). All predominant habitat types have been reported on by at least one Member State. However, only four Member States (BE, DE, FR, UK) have reported on water column habitat types. 
+The pressures reported most often as the main pressures on habitats are physical damage (abrasion) and physical loss (smothering). 
+Species/functional groups 
+Most Member States used a mixed approach to report on species and functional groups. Two Member States reported only on species groups (NL, SE), one Member State reported only on functional groups (PT) and one Member State reported only on individual species (IE). Almost all Member States covered at least birds, fish and mammals. One Member State reported only on fish (IE) and one did not report on mammals due to the lack of sufficient information (PT). However, in a number of cases, not only the information reported did not cover all relevant species/functional groups but the justification provided for the gaps was not considered sufficient (BE, DE, DK, IE). For the majority of Member States, the reports include information on species abundance and condition. The main causes of pressure are also reported but sometimes provide very few details (BE, PT and SE). All Member States provided at least a qualitative/descriptive judgement of the current status of some (e.g. ES and NL) or most (e.g. FR or UK) of the species/functional groups reported. Most Member States referred expressly to the Habitats and Birds Directives (not clear in DK and FR) and to OSPAR or other relevant international conventions (BE, DK and the North Sea subregion in FR are exceptions).
+In the reporting sheets, only one Member State (ES) reported on listed species from the Birds and Habitats Directive (6 species from Birds Directive and 17 from Habitats Directive), despite the agreement that this reporting should be deferred to the 2013 reporting processes under these two Directives. Four Member States (DE, DK, ES, IE) reported on listed species from the OSPAR Convention. 
+With regard to the approach used to report at the species level, five Member States have reported at species group level on birds, fish and mammals (BE, ES, FR (except fish), NL, SE). Three Member States have reported on bird functional groups (BE, DE, DK), four Member States have reported on fish functional groups (BE, DK, FR, UK), three Member States have reported on mammal functional groups (BE, DK, UK) and three Member States have reported on reptiles (turtles) (ES, FR UK). Only one Member State (PT) has reported on (coastal and deep-sea) cephalopods in its initial assessment. 
+The pressures reported most often as the main pressures on species are extraction of species (all species) and biological disturbance (unspecified). 
+Ecosystems
+Only three Member States (DK, ES, NL) have reported on ecosystems. They provided a limited description of the ecosystem structure and its functioning and reported on the main pressures. Only one Member State (DK) provided a conclusive judgement on the current status of its ecosystems. One Member State provided a descriptive judgement (ES) and the other one did not make any judgement on status. 
+In, the reporting sheet, the pressures reported most often as the main pressures on ecosystems are extraction of fish and shellfish and nutrient enrichment.
+Habitats
+While most Member States covered at least a good share of the relevant seabed habitat types, more than half of Member States did not cover, or covered in a very limited way, water column habitat types (BE, DE, DK, ES, IE and NL). The majority of Member States used the MSFD classification of predominant habitats or an equivalent system (in particular EUNIS Level 2 classification), although in some cases the correspondence is not entirely clear (e.g. BE). When assessing habitats, all Member States reported on habitat distribution, extent and condition, as well as on the main causes of pressure (albeit with different levels of detail). However, only three Member States (PT, SE, UK) have provided a clear and conclusive judgement on the current status of the habitats. The Habitats Directive is mentioned by nine out of ten Member States (except DE and the North Sea subregion in FR) as are OSPAR and other relevant international conventions.
+In the reporting sheets, three Member States (BE, DK, ES) reported on listed habitats from the Habitats Directive, despite agreement that this reporting should be deferred to the 2013 reporting processes under these two Directives, and four Member States (DE, DK, ES, IE) reported on listed habitats from the OSPAR Convention. All Member States that have reported (i.e. all Member States from the region minus Portugal) have reported using the MSFD predominant habitat type classification. The predominant habitat types which have been most reported are shallow sand (6 Member States), shelf coarse sediment (6 Member States), shelf mixed sediment (6 Member States) and shallow mud (5 Member States). All predominant habitat types have been reported on by at least one Member State. However, only four Member States (BE, DE, FR, UK) have reported on water column habitat types. 
+The pressures reported most often as the main pressures on habitats are physical damage (abrasion) and physical loss (smothering). 
+Species/functional groups 
+Most Member States used a mixed approach to report on species and functional groups. Two Member States reported only on species groups (NL, SE), one Member State reported only on functional groups (PT) and one Member State reported only on individual species (IE). Almost all Member States covered at least birds, fish and mammals. One Member State reported only on fish (IE) and one did not report on mammals due to the lack of sufficient information (PT). However, in a number of cases, not only the information reported did not cover all relevant species/functional groups but the justification provided for the gaps was not considered sufficient (BE, DE, DK, IE). For the majority of Member States, the reports include information on species abundance and condition. The main causes of pressure are also reported but sometimes provide very few details (BE, PT and SE). All Member States provided at least a qualitative/descriptive judgement of the current status of some (e.g. ES and NL) or most (e.g. FR or UK) of the species/functional groups reported. Most Member States referred expressly to the Habitats and Birds Directives (not clear in DK and FR) and to OSPAR or other relevant international conventions (BE, DK and the North Sea subregion in FR are exceptions).
+In the reporting sheets, only one Member State (ES) reported on listed species from the Birds and Habitats Directive (6 species from Birds Directive and 17 from Habitats Directive), despite the agreement that this reporting should be deferred to the 2013 reporting processes under these two Directives. Four Member States (DE, DK, ES, IE) reported on listed species from the OSPAR Convention. 
+With regard to the approach used to report at the species level, five Member States have reported at species group level on birds, fish and mammals (BE, ES, FR (except fish), NL, SE). Three Member States have reported on bird functional groups (BE, DE, DK), four Member States have reported on fish functional groups (BE, DK, FR, UK), three Member States have reported on mammal functional groups (BE, DK, UK) and three Member States have reported on reptiles (turtles) (ES, FR UK). Only one Member State (PT) has reported on (coastal and deep-sea) cephalopods in its initial assessment. 
+The pressures reported most often as the main pressures on species are extraction of species (all species) and biological disturbance (unspecified). 
+Ecosystems
+Only three Member States (DK, ES, NL) have reported on ecosystems. They provided a limited description of the ecosystem structure and its functioning and reported on the main pressures. Only one Member State (DK) provided a conclusive judgement on the current status of its ecosystems. One Member State provided a descriptive judgement (ES) and the other one did not make any judgement on status. 
+In, the reporting sheet, the pressures reported most often as the main pressures on ecosystems are extraction of fish and shellfish and nutrient enrichment.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the biodiversity descriptors, all Member States but two (IE, PT) have defined environmental targets.  Overall, the level of coherence in the setting of targets and indicators across the North East Atlantic marine region is low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the biodiversity descriptors, all Member States but two (IE, PT) have defined environmental targets. 
+Two Member States (FR, SE) have defined separate targets for D1, D4 and D6. For these two, the number of targets is rather limited (between four (SE) and seven (FR)) but associated with indicators. The other six Member States (BE, DE, DK, ES, NL, UK) have addressed with one set of targets the three descriptors. In these cases, targets are grouped according to the ecosystem level they address (i.e. habitat, species or ecosystem). The number of targets is generally high for these countries, from 12 (NL) to more than 30 (UK). 
+The biodiversity targets represent a mix of state, impact and pressure targets, with a domination of state and impact targets. The pressures addressed are mainly those related to fishing activities and/or causing physical damage to the seafloor (including selective extraction of species, bottom trawling, by-catch, discards, etc.). Two Member States have not included pressure-targets at all (SE, FR). 
+The Member States that have defined detailed targets have often addressed specific species (except ES) that are considered either sensitive/threatened and in need of protection (e.g. listed species from the Habitats and Birds Directive or from the OSPAR Convention), that have a particular function/ role in the ecosystem (e.g. long-lived, slowly-reproducing species, top predators, etc.), that are particular sensitive to certain pressures (e.g. noise, by-catch, contaminants) or that are well-studied and monitored. Examples of such species commonly addressed by the targets are seals and harbour porpoises (BE, DK, NL).
+Most Member States have addressed the main three species groups in their targets: fish, birds, mammals. One Member State (SE) has focused only on fish. Within the targets on fish, only a limited number of Member States (ES, NL) have addressed elasmobranchs (sharks, skates, rays, etc.). Only one Member State (ES) covers reptiles in its targets and none cover cephalopods. 
+In terms of quantification, only three Member States (BE, NL, UK) have defined thresholds and baselines for their targets and indicators (and most of the time only for a selection of targets). A lot of Member States have defined quantitative parameters but without providing threshold values that allow to measure the achievement of the target (e.g. DK, ES, SE). Some Member States (NL, UK) have explained that while they did not reproduce the standards found in other legislation (e.g. WFD, HBD) in their targets, these apply where relevant. 
+Only four Member States out of ten have used, or referred to, OSPAR EcoQOs as associated indicators for their targets (BE, NL, UK) or as general reference levels (DE). 
+For the biodiversity descriptors, all Member States but two (IE, PT) have defined environmental targets. 
+Two Member States (FR, SE) have defined separate targets for D1, D4 and D6. For these two, the number of targets is rather limited (between four (SE) and seven (FR)) but associated with indicators. The other six Member States (BE, DE, DK, ES, NL, UK) have addressed with one set of targets the three descriptors. In these cases, targets are grouped according to the ecosystem level they address (i.e. habitat, species or ecosystem). The number of targets is generally high for these countries, from 12 (NL) to more than 30 (UK). 
+The biodiversity targets represent a mix of state, impact and pressure targets, with a domination of state and impact targets. The pressures addressed are mainly those related to fishing activities and/or causing physical damage to the seafloor (including selective extraction of species, bottom trawling, by-catch, discards, etc.). Two Member States have not included pressure-targets at all (SE, FR). 
+The Member States that have defined detailed targets have often addressed specific species (except ES) that are considered either sensitive/threatened and in need of protection (e.g. listed species from the Habitats and Birds Directive or from the OSPAR Convention), that have a particular function/ role in the ecosystem (e.g. long-lived, slowly-reproducing species, top predators, etc.), that are particular sensitive to certain pressures (e.g. noise, by-catch, contaminants) or that are well-studied and monitored. Examples of such species commonly addressed by the targets are seals and harbour porpoises (BE, DK, NL).
+Most Member States have addressed the main three species groups in their targets: fish, birds, mammals. One Member State (SE) has focused only on fish. Within the targets on fish, only a limited number of Member States (ES, NL) have addressed elasmobranchs (sharks, skates, rays, etc.). Only one Member State (ES) covers reptiles in its targets and none cover cephalopods. 
+In terms of quantification, only three Member States (BE, NL, UK) have defined thresholds and baselines for their targets and indicators (and most of the time only for a selection of targets). A lot of Member States have defined quantitative parameters but without providing threshold values that allow to measure the achievement of the target (e.g. DK, ES, SE). Some Member States (NL, UK) have explained that while they did not reproduce the standards found in other legislation (e.g. WFD, HBD) in their targets, these apply where relevant. 
+Only four Member States out of ten have used, or referred to, OSPAR EcoQOs as associated indicators for their targets (BE, NL, UK) or as general reference levels (DE). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for Descriptor 4 for all their marine waters, not distinguishing between subregions. The level of coherence across the North East Atlantic marine region for the definition of Good Environmental Status for Descriptor 4 is low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None of the ten Member States of the North East Atlantic marine region have defined GES for Descriptor 4 the same way. One Member State (NL) has just reproduced verbatim the text of Annex I of the MSFD. A majority of Member States (BE, DK, ES, FR, SE, UK) have defined GES for D4 at the level of the criteria, although for two of these Member States (DK, UK) the coverage of the Commission Decision criteria is implicit rather than explicit.  One Member State (IE) has defined GES for criteria 4.1 and 4.3 only. One Member State (PT) has defined GES for D4 at a very high, general level and the last Member State (DE) has provided a global definition for D1, D4 and D6, which is only tenuously related to D4.
+Some Member States have defined GES in such a way that it covers all food-web components indiscriminately (i.e. from plankton to higher trophic levels) (BE, ES, FR, NL, PT, SE), whether because the GES definition is very general (NL, PT) or because it includes a general statement which addresses all food webs in holistic manner (BE, ES, FR, SE). Most Member States have referred to specific food web components in their GES definition, sometimes in addition to defining it for all food web components. Most Member States (BE, DK, ES, FR, IE, SE, UK) refer to ‘key’ species or functional groups, some also refer to top predators or species at the top of the food web (BE, FR, SE). Two Member States (DK, SE) also included specific species as indicators of change in their GES definition, including the harbour porpoise and the harbour seal. 
+Only two Member States (ES, UK) have included a reference to the pressures on food web components, in particular fisheries (e.g. by-catch and discards). 
+Only three Member States (BE, SE, UK) have specified a baseline for their GES definitions, and it is clearly defined only for two of these three Member States (BE, SE). Only one of the two Member States (SE) has defined its baseline as ‘reference conditions’, i.e. in line with prevailing conditions. For the third Member State (UK), baselines are defined for specific indicators/species. Similarly, only three Member States have provided threshold values for certain criteria/indicators/species. A number of Member States (BE, DK, ES, FR, UK) however refer to the “maintenance” of various criteria/indicators (e.g. of the productivity of key trophic groups) but it is not clear whether it is maintenance in relation to a current status. Most add that these indicators should be maintained so as to ensure the long-term sustainability of populations and the balance of the food web. 
+Only two Member States (ES, FR) include energy transfers between trophic levels in their GES definition. A third Member State (UK) acknowledges the gap with regard to this aspect, justifying that there is a lack of knowledge to meaningfully cover this aspect of the Descriptor. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The level of coherence of the initial assessments on physical damage and loss across the North East Atlantic marine region is relatively high. 
+All Member States have undertaken an initial assessment on physical loss and physical damage.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have covered most types of physical loss and physical damage. Likewise, all Member States have covered the main causes of pressure albeit at different levels of detail. Thus, while two Member States (ES, PT) report comprehensively on each type of pressure, including quantifying some parameters, in other Member States (e.g. BE, UK) the information focuses only on certain types of pressures and is more limited. The impacts of physical loss and physical damage are also covered by all Member States although some have not covered them in much detail (DE, IE, NL, SE). 
+Member States refer expressly to WFD reports (e.g. BE and IE) or to OSPAR relevant documents (e.g. DK and IE). Only one Member State (DK) presented clear conclusive judgements on the level of pressure of physical loss and physical damage and their impacts.
+In the reporting sheets, half of the Member States (BE, DK, ES, IE, NL) report that less than 1% of their assessment area (and of their seabed habitats) is affected by physical loss. The other Member States (DE, FR, SE, UK) do not report anything. For physical damage, there is more variation as one Member State (ES) reports that less than 1% of its assessment area is affected, two Member States (IE, UK) report 5-25%, one Member State (SE) reports 50-75% and three Member States (BE, DK, NL) report that 75 to 100% of their assessment area (and seabed habitats) is affected. The other Member States (DE, FR) do not report anything. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitats
+While most Member States covered at least a good share of the relevant seabed habitat types, more than half of Member States did not cover, or covered in a very limited way, water column habitat types (BE, DE, DK, ES, IE and NL). The majority of Member States used the MSFD classification of predominant habitats or an equivalent system (in particular EUNIS Level 2 classification), although in some cases the correspondence is not entirely clear (e.g. BE). When assessing habitats, all Member States reported on habitat distribution, extent and condition, as well as on the main causes of pressure (albeit with different levels of detail). However, only three Member States (PT, SE, UK) have provided a clear and conclusive judgement on the current status of the habitats. The Habitats Directive is mentioned by nine out of ten Member States (except DE and the North Sea subregion in FR) as are OSPAR and other relevant international conventions.
+In the reporting sheets, three Member States (BE, DK, ES) reported on listed habitats from the Habitats Directive, despite agreement that this reporting should be deferred to the 2013 reporting processes under these two Directives, and four Member States (DE, DK, ES, IE) reported on listed habitats from the OSPAR Convention. All Member States that have reported (i.e. all Member States from the region minus Portugal) have reported using the MSFD predominant habitat type classification. The predominant habitat types which have been most reported are shallow sand (6 Member States), shelf coarse sediment (6 Member States), shelf mixed sediment (6 Member States) and shallow mud (5 Member States). All predominant habitat types have been reported on by at least one Member State. However, only four Member States (BE, DE, FR, UK) have reported on water column habitat types. 
+The pressures reported most often as the main pressures on habitats are physical damage (abrasion) and physical loss (smothering). 
+Species/functional groups 
+Most Member States used a mixed approach to report on species and functional groups. Two Member States reported only on species groups (NL, SE), one Member State reported only on functional groups (PT) and one Member State reported only on individual species (IE). Almost all Member States covered at least birds, fish and mammals. One Member State reported only on fish (IE) and one did not report on mammals due to the lack of sufficient information (PT). However, in a number of cases, not only the information reported did not cover all relevant species/functional groups but the justification provided for the gaps was not considered sufficient (BE, DE, DK, IE). For the majority of Member States, the reports include information on species abundance and condition. The main causes of pressure are also reported but sometimes provide very few details (BE, PT and SE). All Member States provided at least a qualitative/descriptive judgement of the current status of some (e.g. ES and NL) or most (e.g. FR or UK) of the species/functional groups reported. Most Member States referred expressly to the Habitats and Birds Directives (not clear in DK and FR) and to OSPAR or other relevant international conventions (BE, DK and the North Sea subregion in FR are exceptions).
+In the reporting sheets, only one Member State (ES) reported on listed species from the Birds and Habitats Directive (6 species from Birds Directive and 17 from Habitats Directive), despite the agreement that this reporting should be deferred to the 2013 reporting processes under these two Directives. Four Member States (DE, DK, ES, IE) reported on listed species from the OSPAR Convention. 
+With regard to the approach used to report at the species level, five Member States have reported at species group level on birds, fish and mammals (BE, ES, FR (except fish), NL, SE). Three Member States have reported on bird functional groups (BE, DE, DK), four Member States have reported on fish functional groups (BE, DK, FR, UK), three Member States have reported on mammal functional groups (BE, DK, UK) and three Member States have reported on reptiles (turtles) (ES, FR UK). Only one Member State (PT) has reported on (coastal and deep-sea) cephalopods in its initial assessment. 
+The pressures reported most often as the main pressures on species are extraction of species (all species) and biological disturbance (unspecified). 
+Ecosystems
+Only three Member States (DK, ES, NL) have reported on ecosystems. They provided a limited description of the ecosystem structure and its functioning and reported on the main pressures. Only one Member State (DK) provided a conclusive judgement on the current status of its ecosystems. One Member State provided a descriptive judgement (ES) and the other one did not make any judgement on status. 
+In, the reporting sheet, the pressures reported most often as the main pressures on ecosystems are extraction of fish and shellfish and nutrient enrichment.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for Descriptor 6 for all their marine waters, not distinguishing between subregions. The level of coherence across the North East Atlantic marine region for the definition of Good Environmental Status for Descriptor 6 is low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None of the ten Member States of the marine region have defined GES the same way and the vast majority of the Member States sharing North-East Atlantic waters have defined GES for Descriptor 6 in a rather vague way. The majority of Member States (BE, DK, ES, FR, IE, PT, SE) have defined GES for Descriptor 6 at criteria level. Most of these (BE, DK, ES, FR, SE) have defined GES for both criteria of the Commission Decision, 6.1 and 6.2. One Member State has covered only 6.1 (PT) and the other only 6.2 (IE). One Member State (NL) has simply reproduced verbatim the text of Annex I of the MSFD and another Member State (UK) has defined GES only at descriptor level. One Member State (DE) has provided a joint definition with Descriptor 1 and 4 however the definition only has a tenuous link to Descriptor 6.
+In terms of indicators, a few Member States have included some of the Commission Decision indicators in the scope of their GES definitions, in particular those under criterion 6.1. A majority of Member States (DK, ES, FR, NL, PT, SE) refer to the reduction of physical pressures from human activities on the seabed, either directly or indirectly (through reference to impacts). However, only one Member State (FR) has included a quantitative indicator on the percentage of area occupied by biogenic substrate acted upon by human pressures but has not specified a threshold value. 
+Criterion 6.2 on the condition of the benthic community is hardly ever specified through indicators. Only one Member State (SE) has included a quantitative indicator, the Benthic Quality Index, related to indicator 6.2.2 and to the Water Framework Directive. Only two other Member States (BE, DE) refer to the WFD good ecological status. The definitions for 6.2 of the other Member States are generally vague despite the fact that the condition of the benthic community is one of the most studied and well-documented aspect of biodiversity across most of Europe, for which a number of WFD indicators could have been used.  
+None of the Member States have specified substrate types covered by their GES definition. Only one Member State (FR) refers to the specific habitats selected for D1 and two Member States (BE, DE) refer to protected/listed habitats and constituent species. The same three Member States (BE, DE, FR) have referred to OSPAR but only one (FR) to the OSPAR advice on D6.  
+Only three Member States (BE, DK, IE) mention a baseline, two (DK, IE) use it in the sense of reference/ prevailing conditions and one (BE) uses the current status (2012 initial assessment) as the baseline. None of the Member States use the WFD principle of ‘reference conditions plus acceptable deviation’. 
+A number of Member States (ES, SE, UK) mention the need to maintain the status and integrity of the seafloor habitats to ensure their long-term/sustainable functioning. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for all their marine waters, not distinguishing between subregions. Overall, the level of coherence with regard to D2 in the North East Atlantic Ocean region is considered as low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The large majority of the Member States sharing North-East Atlantic waters have defined GES in a rather vague way. Two Member States (NL, PT) simply reproduce verbatim or very closely the definition of Annex I. Amongst the other Member States, there are major differences as to the level of details and focus. Several Member States explicitly take a risk-based approach, addressing primarily vectors and pathways (ES to a lesser extent, IE, UK), while others refer to impacts (BE, DE, ES, FR, SE). Only one Member State (ES) considers one specific type of invasive NIS (macroalgae) in its definition. The GES definitions address NIS in general (BE, DE, IE, NL, PT) or only invasive NIS (DK) or both (ES, FR, SE, UK). GES is generally defined at descriptor level, more rarely at criteria level and generally for criterion 2.1 (abundance and state characteristics). 
+One Member State (BE) specifically excludes from its GES definition species for which there are taxonomic disputes and for which the changes following permanent introduction, including reproduction are negligible.
+One Member State (SE) refers to GMOs and species with altered genetic characteristics within its definition of GES.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have undertaken an initial assessment for D2.  The level of coherence is considered as high. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The initial assessment for D2 is, as a rule, based on existing literature or, in certain cases, expert judgement. All Member States have provided an inventory of NIS present in their marine waters. Only one Member State (SE) has focused only on the most important invasive species. The main vectors and pathways are generally described. The assessment of impacts remains limited. When the level of pressure is provided, it is in a qualitative way. Only three Member States (BE, DE, PT) have indicated a trend in the level of pressure and only one (PT) has made a judgement of the pressure albeit with a low level of confidence. On the whole, Member States describe in detail knowledge and data gaps and, more rarely, plans to address them, but often with limited detail.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For D2, almost all Member States have defined environmental targets and associated indicators for all their marine waters, not distinguishing between subregions. The only exception is Portugal which has not set environmental targets for D2. In conclusion, the level of coherence is low across the North East Atlantic region in terms of environmental targets and associated indicators.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of targets varies from 1 to 4. A few countries have set interim targets but most targets express GES. Only one Member State (SE) has set a state target. All other Member States have set pressure/impact targets. However, the targets rarely mention specific vectors/pathways (DK, ES, IE, SE) or specific NIS (ES). The level of details varies greatly from one Member State to another. None of the environmental targets have been assessed as fully SMART, often because they are not measurable.
+All the Member States have set targets relating to the reduction of new introductions of NIS (BE, DE, ES, FR, IE, NL, SE, UK), sometimes also mentioning spreading (ES, FR, IE, UK). One Member State has set targets only focusing on prevention of NIS transport by shipping and aquaculture (DK). The way this type of target on minimisation of new introductions is further specified differs from one Member State to another. While some Member States bring little or no specification (BE, FR, NL), others give more details, sometimes restricting the target e.g. to macro-fauna and flora above 1 mm (BE) or specifying which type of measures should be taken (DE, IE, UK) or which vectors/pathways should be addressed (ES, SE). Two Member States (FR, UK) addresses in addition the reduction of impacts from NIS but their target is formulated in a very general way.
+The associated indicators vary even more, with two Member States who have not set associated indicators (BE, FR) . Several Member States refer to the number of newly introduced NIS (DE, SE).
+Several Member States refer to the number of (invasive) NIS in various ways e.g. screening of abundance, occurrence in risk areas for selected invasive species (DK), focusing on areas which are at high risk of new introductions (UK) or Natura 2000 sites or international ports and major shipping routes (SE), or in a more general way e.g. number of invasive NIS (ES). One Member State (NL) set indicators for both the number of invasive NIS present and the number of newly-introduced species.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States with marine waters in the North-East Atlantic marine region have defined GES for Descriptor 3. Overall, the level of coherence for the definition of GES for D3 across the Member States of the North East Atlantic marine region is considered to be moderate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Four Member States have defined GES only at the descriptor level (DK, IE, NL, PT). Out of these, one has provided a verbatim copy of the descriptor from Annex I of the MSFD (NL) while two have provided a GES definition that is close to the Annex I definition but in an undetailed way incorporates some aspects of criteria 3.1 of the Commission Decision (IE, PT). Finally one Member State has provided a general statement which should correspond to definition at descriptor level but is less specific than the definition as provided in Annex I MSFD (DK). The remaining Member States have all applied criteria 3.1 and 3.2 and three out of those six Member States have applied criterion 3.3 from the Commission Decision (DE, FR, SE). 
+In regard to criteria 3.1 all Member States that have clearly defined criteria 3.1 have used F as the primary indicator and each of those have used Fmsy in their GES definition. Only one however has clearly stated that all fish and shellfish should be exploited at or below Fmsy (DE) while another has clearly set this threshold for all exploited fish species (SE). The remaining countries have GES definitions which do not require either explicitly or implicitly that all stocks are exploited at or below Fmsy. Two Member States have used Fmsy as being target values rather than limits (ES, FR). For those stocks for which F cannot be determined, a number of Member States have applied the secondary indicator 3.1.2 from the Commission Decision, the catch/biomass ratio (BE, DE, FR, SE). One Member State has also provided a third indicator using catch per unit effort (CPUE) (BE). 
+For criteria 3.2, all six Member States who have defined GES beyond the descriptor level have applied the primary indicator SSB. Two Member States have explicitly defined SSBpa as a threshold for some or all stocks (BE, DE) and four implicitly apply PA levels by stating that stocks need to be within safe biological limits (IE, NL, SE, UK) in their GES definition. Two Member States also apply additional reference points which are to be used as the primary indicator for measuring the achievement of GES, one uses SSBmsy (BE) and one BMSY-Btrigger (DE). These countries apply SSBpa when the other proxy is not known. Two Member States (FR, SE) only used BMSY-trigger for defining the threshold for indicator 3.2.1. In some Member States, it is less clear that all stocks should be within safe biological limits due to specificities within the GES definitions (UK, SE). Furthermore two Member States clearly deviate from the others in their setting of criterion 3.2 (ES, FR). In order to achieve GES, one (FR) requires all assessed stocks to have a reproductive biomass at or above MSY-Btrigger with a probability of 50%. The other (ES) deviates from the other North-East Atlantic countries by setting GES as being achieved when SSB/SSBmsy ≥1 for at least 50% of the stocks and not &lt;0.6 to any stock, instead of using SSBpa reference points. Two Member States have used the secondary indicator of the Commission Decision 3.2.2 Biomass indices (SE, FR) and one proposes using the indicator in their GES (DE). One Member State proposes another indicator using the trends of survey abundance as a proxy for stock biomasses (BE).
+Guidance for criterion 3.3 is still less developed than that for criteria 3.1 and 3.2 and only three out of the ten Member States of the marine region have defined a criterion with associated indicators that corresponds to criterion 3.3 of the Commission Decision (DE, FR, SE). One Member State has applied all four indicators from the Commission Decision verbatim (DE). Another one has applied indicator 3.3.1 with a threshold and applied indicator 3.3.3 without a threshold (FR). The last one has defined two indicators for criteria 3.1 which are more closely aligned to criteria 3.3 (SE). These are not verbatim copies of the Commission Decision; a threshold value has even been set for one of the two indicators. Criterion 3.3 is the least developed criterion for Descriptor 3 within the North East Atlantic marine region. None of the GES definitions within the North East Atlantic marine region are directly comparable but none have used a descriptor, criterion or indicator in a way that significantly deviates from those provided in the Commission Decision (except for Spain for criterion 3.2). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have undertaken an initial assessment for D3. In general, the level of coherence of the initial assessments undertaken by Member States in the North-East Atlantic marine region is considered to be moderate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The North-East Atlantic countries have used ICES MSY and PA reference points but within the countries there are differences in the reference points used. A majority of Member States have assessed stocks in relation to the Fmsy reference point (ES, FR, IE, PT, SE, UK) while one has assessed stocks in relation to fishing mortality F but it is unclear which reference point has been applied (NL). Two Member States have not sufficiently specified which ICES reference points were used to assess the status of their fish and shellfish stocks (DE, NL).
+Two Member States have assessed the spawning stock biomass in relation to the SSBpa reference points (FR, UK), one has implicitly done so by using the OSPAR EcoQO which requires stocks to be above SSBpa (BE). Another one has used the BMSY-trigger as a reference point to assess stocks (DK) while two have assessed stocks in relation to the SSBmsy reference points (ES, SE). Finally, one Member State has used both SSBmsy and BMSY-trigger reference points (PT).
+Two Member States have also used comparisons of recently observed fishing mortality F and SSBs to historical trends to assess the status of stocks (ES, PT). 
+Two Member States in the marine region have not assessed the status shellfish stocks (BE, SE). 
+In terms of impacts on seabed habitats, only four Member States have provided, in the reporting sheets, a quantification of the extent of the seabed affected by the fishing pressure. This figure however varies quite widely, from 5-25% in one Member State (UK) to 75-100% in another (DE) with another two reporting 50-75% (DK, NL). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For D3, all Member States have defined environmental targets and associated indicators for all their marine waters, not distinguishing between subregions.  Overall, the level of coherence in the setting of targets for D3 across the North-East Atlantic marine region is low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two countries have clearly stated in their targets that all stocks should be exploited at or below Fmsy (NL, UK) and both have explicitly stated that in order for the target to be achieved, all stocks should be at Fmsy, while another has set Fmsy as a limit, but it is unclear whether this applies to all stocks (SE). Four countries have set as their targets that all stocks are managed according to MSY principles (BE, DE, DK, IE). One Member State has only set specific targets for three stocks to be exploited at MSY by 2015 or at the latest by 2020 (PT) and two Member States have not set any targets explicitly or implicitly using Fmsy (ES, FR). 
+In regard to secondary indicators of the Commission Decision for fishing mortality, two Member States have applied the secondary indicator 3.1.2 catch biomass ratio (DE, SE) while two others have applied the catch per unit effort (CPUE) (BE, NL). Three Member States have not clarified which secondary indicators they intend to use (DK, FR, UK).  
+The same three Member States have set as a target for all stocks to be at SSBpa (BE, NL, UK) while one implicitly does so by requiring all commercial species to be within safe biological limits (ES). One Member State has set as a target for all stocks to be at a level higher than BMSY-trigger (SE). Another one has set SSBpa as a target for its stocks but it is not clear whether achievement of the target requires all stocks to be at PA levels (DK). Three Member States have not set any targets for stocks to be at or above SSBpa levels (DE, FR, PT). Only one Member State has set as a target for all stocks to be at Bmsy (BE). Furthermore one Member State within the North-East Atlantic region has applied specific targets relating to the biomass recovery of specific species (PT). 
+Four out of ten Member States have defined associated indicators for the GES indicators of criterion 3.3 of the Commission Decision. Only one Member State has a target which is similar to the GES definition as provided in Annex I of the MSFD and contains the text “with an age (when available) or size (if ages not available) distribution indicative for a healthy stock” which could correspond to criterion 3.3 of the Commission Decision (BE). Two Member States provide indicators, which relate to, but are not exact copies of, the indicators provided in the Commission Decision for criterion 3.3 (DE, SE). Some Member States have applied verbatim copies of the Commission Decision indicators for criterion 3.3 (3.3.3 for NL, 3.3.1, 3.3.3 and 3.3.4 for IE). None of the indicators contain thresholds and there is no use of the OSPAR EcoQOs. Targets related to criterion 3.3 can be considered at a very low stage of development within the North Sea region. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for Descriptor 5. Overall, the level of coherence in the North East Atlantic marine region for D5 is relatively high.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practically all Member States have covered all three criteria of the Commission Decision in their GES (the case of the Netherlands is not entirely clear). In relation to the inclusion of the Commission Decision indicators the situation is not homogenous. One Member State (FR) has clearly covered all the indicators, but in any case the majority of Member States covered most of the indicators. There are two indicators which are excluded most systematically than the others: indicator 5.1.2 (nutrient ratios) and 5.2.2 (water transparency). While most Member States have included criteria relating to both pelagic and seabed habitats, some seem not to cover seabed (macrophytobenthos) communities (BE, NL, PT, UK). Two Member States (e.g. ES, FR) state that GES for D5 can be achieved even if nutrient levels are higher than thresholds values, providing there are no direct or indirect impacts, but this does not appear to be the predominant view.
+Practically all Member States refer to the appropriate normative definitions of ecological status classifications of the Water Framework Directive (WFD) for coastal waters but the relation between the MSFD GES and the WFD GES is not always completely clear (e.g. DK). Only one Member State has been very specific about using WFD thresholds for good/high status to define MSFD GES in those coastal waterbodies currently achieving High Ecological Status under the WFD (IE). Reference to the OSPAR approach is also mentioned either in the definition of GES or in the accompanying text of practically all Member States. All countries appear to have produced GES definitions which allow them to re-use data already gathered, or continuing to be collected for OSPAR and WFD purposes. Taking this a step further, certain Member States have defined GES in terms of achieving OSPAR eutrophication non-problem status (DE, IE, UK). Most countries appear to have adopted the OSPAR nutrient baseline/threshold levels for offshore waters at least (exceptions include DK, NL and PT; the case of the UK is not completely clear). Depending on WFD normative classifications, there appears to be a mixture of WFD-based chlorophyll and nutrient thresholds and OSPAR-derived thresholds used for coastal waters, although the OSPAR-derived thresholds take account of WFD coastal water thresholds. With regard to changes in floristic composition, there appears to have been little reference to benthic-pelagic shifts, but reference to OSPAR’s phytoplankton indicator species appears to be more common (e.g. DE, IE). In line with OSPAR’s Comprehensive Procedure, a limited number of countries (e.g. SE) appear to judge indirect impacts on the zoobenthos community using an invertebrate index, in addition (or as an alternative) to dissolved oxygen status. 
+The vast majority of Member States did not incorporate quantitative thresholds in their definition of GES and therefore it is not always easy to know when GES is actually achieved. Ireland and Sweden are clear exceptions. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have undertaken an initial assessment for D5.Overall, the level of coherence in the initial assessment of nutrient and organic matter enrichment is high in the North East Atlantic marine region.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States provided the loads of the relevant nutrients – nitrogen and phosphorus – and a majority of them have also provided their concentrations in the environment. A certain number of Member States, however, have not provided much information on organic matter inputs (BE, DE, ES, UK).
+There appears to be further differences in knowledge with regard to nutrient (and organic) source apportionment. While most countries appear to have a reasonable or good understanding of where those nutrients/organic matter originate from, quantification of the original source loads is usually lacking (e.g. IE). This is particularly the case where fluvial fluxes predominate, the relative contributions of point vs. diffuse sources to river loads remain unclear. In terms of nutrient loading, riverine and atmospheric inputs are usually considered, but some countries do not appear to have considered direct discharges (BE, FR, UK). Groundwater inputs (of nitrate) do not appear to have been considered by any North East Atlantic Member States while these may represent significant localised inputs in some areas at least.
+The age of data used to calculate loads also varies substantially, with some relying on data sometimes more than 10 years old (FR). There appears to be an inconsistency over the inclusion of WFD phytobenthos data for assessing inter-tidal/infralittoral aquatic vegetation. Some countries appear to have used it (DK), while others do not (UK, SE). There is generally a dearth of phytobenthos results for offshore waters which, for many Member States, will be genuine (the seabed is lower than the euphotic zone). For other Member States with extensive shallow shelf areas, it is not clear whether phytobenthos communities exist or not. The limited amount of phytobenthos data/information has meant that changes in floristic composition are considered overwhelmingly in the light of OSPAR phytoplankton indicator species. No Member State has provided information on benthic-pelagic shifts. All countries have presented a judgement on trophic status pressure and/or impact trends even if not always per reference to GES (e.g. for FR or UK).
+Although not part of the Commission Decision requirements, benthic invertebrate status is used by some MSs (e.g. France in its Bay of Biscay waters) to assist in assessing dissolved oxygen impacts. Only one Member State (IE) has considered in its initial assessment both low dissolved oxygen as an indicator of eutrophication impacts and oxygen supersaturation (values &gt; 130%) as an indicator of elevated phytoplankton photosynthesis. 
+In the reporting sheets, only half of the Member States (DE, DK, IE, NL, UK) have provided a quantification of the proportion of the water column which is impacted by nutrient and organic matter enrichment. These figures vary quite widely from one Member State to another, with two Member States (IE, UK) reporting less than 1% of their water column habitats as impacted, one (NL) reporting 5-25%, one (DK) reporting 25-50% and the last (DE) reporting that 75-100% of its water column habitats are impacted by nutrient and organic matter enrichment. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For D5, all Member States in the North East Atlantic marine region have defined environmental targets and associated indicators for all their marine waters, not distinguishing between subregions (except France). The only exception is PT which has not set environmental targets for D5.Overall, the level of coherence in the setting of targets for D5 across the North East Atlantic marine region is moderate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most Member States fall into one of two broad groups. The targets set by a first group (BE, DK, IE, NL, SE) are all state/impact based, effectively representing the achievement of GES, albeit without timescales. The targets set by a second, smaller group of Member States (DE, ES, FR) are usually qualitative targets, less ambitious, principally concerned with either reducing nutrient loads (pressure-based) to the marine environment or conserving areas with little or no eutrophication impacts (no deterioration targets). 
+In an additional approach to the above eight countries, one Member State (UK) has adopted a risk (and state/impact)-based) approach to target setting, providing greater numbers of targets for known eutrophication-impacted areas (OSPAR-recognised eutrophication problem areas) than for non-impacted areas. In stark contrast to all of the above, one Member State (PT) has reported one generic target on monitoring which is applicable to D5. The target presented is very broad and not specific to eutrophication.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for D7. Overall, the level of coherence in the definitions of GES for D7 across the North East Atlantic marine region is high.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All MSs use the same baseline (present) and most of them consider that their waters are at GES for D7 (but often based on lack of knowledge rather than on their Initial Assessment). Most countries have determined GES at general level (only at descriptor level, or including criteria but without specifying scale, indicator, habitats, species and ecosystems) (BE, DE, DK, ES, NL, PT, UK). Beyond this general determination, which is usually close to the MSFD Annex I definition of GES, only some countries have specified the environment components to be taken into account and given a list of relevant parameters (FR) or activities (IE).
+Only one Member State (DE) has established a clear link to WFD normative definitions of ecological status classifications for coastal waters. The fact that none of the other Member States has done this is a gap in comparison to the OSPAR Advice document on Hydrographical conditions (MSFD Descriptor 7) or the Commission Staff Working Paper on the Relationship between the initial assessment of marine waters and the criteria for good environmental status (SEC(2011) 1255 final)  and is not coherent with the general assessment that most pressures related to D7 occur in coastal zones. However, some Member States do refer to other existing regulatory regimes to be complied with (e.g. EIA, SEA, Habitats and Birds Directives) (FR, IE, NL, UK).
+The OSPAR advice has generally been used only partially and usually in its restrictive considerations: focus on new activities only (this is clearly the case for FR and NL). Some MSs clearly refer to the list of potentially impacted environment components, linking D7 to D1, D4 and D6 (FR, IE, SE, UK). Few countries (e.g. FR) explicitly refer to plans in order to improve GES D7 definition, or even refer to the actions already proposed in OSPAR Advice.
+None of the Member States incorporate clear quantitative thresholds in their definition of GES. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have undertaken an initial assessment for D7. The level of coherence of the initial assessments on hydrological process across the North East Atlantic is moderate, despite the important recent work done at OSPAR level for nearly all subregions (QSR 2010).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A number of countries (e.g. FR, NL) refer to (or use without clear reference) the OSPAR QSR 2010. Some countries seem to have produced less detailed reports, focused only on some areas (coastal) and with missing elements such as impacts on specific environment components (BE, ES, IE, UK); this is often based on the hypothesis that present status is at GES, which is assumed but not clearly demonstrated. Some have produced a very basic and general assessment, without proper analysis of pressures and impacts and focused only on some parameters (usually temperature and salinity, sometimes currents) (DE, DK, SE). Plans to address the existing knowledge gaps are provided by some Member States (DE, ES, FR, IE, UK). Few countries explicitly refer to WFD reports (the clear exceptions are again FR and NL), while on the other hand nearly all of them focus on the coastal zones. Most countries report, in the reporting sheets, that less than 1% of their assessment area is affected by hydrological processes. 
+Marine acidification is expressly mentioned, even if in some cases briefly, only by a few Member States (DE, IE, NL, UK). Out of these, three Member States indicate, in the reporting sheets, that 75 to 100 % of their assessment area is affected by marine acidification.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For D7, almost all Member States have defined environmental targets and associated indicators for all their marine waters, not systematically distinguishing between subregions. Denmark and Portugal have not set environmental targets for D7. Overall, the level of coherence in the setting of environmental targets for D7 across the North East Atlantic marine region is high. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most of the MSs (in line with OSPAR Advice) assume that their waters are at GES already and most of the environmental targets defined (when applicable) focused on EIA and SEA for new projects (BE, ES, IE, NL, UK). Other countries have defined general environmental targets more related to the GES definition than to operational targets for D7 (e.g. DE, FR). One Member State (PT) has only reported one generic target on monitoring which is applicable to D7. The target presented is very broad and not specific to hydrographical conditions.
+All Member States have reported impact-based targets but practically none of them have also reported clear pressure-based targets (ES is one exception). No Member State has made a clear link to the WFD objectives or defined clear thresholds.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for Descriptor 8 for all their marine waters, not distinguishing between subregions.  Most Member States have defined GES in a specific way for the two criteria of the Commission Decision: concentration and effects of contaminants. Only three countries have not defined GES for both criteria of the Decision (DK, NL, PT). The level of coherence in the definitions of GES for D8 across the North East Atlantic marine region is relatively high, with a higher level of coherence in the North of the marine region than in the South.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All countries, except the three previously mentioned, have referred to the three possible matrices for measurement of contaminant concentrations (water, biota and sediment). Almost all countries (except DK and ES) have, directly or indirectly, included compliance to the Environmental Quality Standards (EQS) Directive as a requirement to achieve GES. One Member State (UK) has even mentioned its on-going revision. One Member State (NL) has simply referred to the WFD as one of the policies already in place relevant for this descriptor. Finally, one Member State (PT) talks only about “established reference conditions” without further details. Six Member States out of ten (BE, DE, ES, FR, IE, UK) have included a direct or indirect reference to the OSPAR Environmental Assessment Criteria (EACs). For the Member States that apply both the EQS and the EAC, none has explained which approach they will use for the three substances for which both EQS and OSPAR’s EAC apply (Hg, HCB and HCBD in biota). Only one Member State (DE) has mentioned potential issues of complementarity and the need to apply the precautionary principle (NL has also done it in their targets) but without setting a clear hierarchy between the two approaches. 
+Only two countries (FR, SE) have been specific with regard to the substances covered by their GES definition: one covers all priority substances and additional ones (FR), while the other covers only a selection of priority substances (SE). For the other countries, reference to the EQS may mean that all priority substances are covered but there is a lack of specification. One Member State (DE) has included radionuclides in the scope of its GES definition.
+Only two Member States have defined aggregation rules (ES, PT) and one additional Member State (FR) states that they should be defined later, leaving open the question whether the “all in, all out” rule should apply to all the other Member States. 
+Most countries have, directly or indirectly, used OSPAR’s ecological quality objectives (EcoQOs) or OSPAR’s EAC (and/or Effects Range Low values, ERLs) for biological effects of contaminants (BE, DE, ES, FR, IE, SE, UK). However, only one Member State (FR) has made a direct reference to imposex in its GES definition, which is the only mandatory effect adopted by OSPAR. Only two Member States (DE, FR) refer directly to the EcoQO on oiled guillemots. Finally, only three countries (DE, FR, SE) have included a provision on the frequency and/or extent of acute pollution events. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have undertaken an initial assessment for D8. A majority of Member States (DE, DK, ES, FR, IE, PT, SE, UK) have provided a detailed, quantitative, assessment of the level of contamination. All Member States have provided a list of the contaminants considered in their assessment. The most common man-made substances assessed include PCBs, PAHs, TBT, DDT and the most common heavy metals assessed include cadmium, lead and mercury (identified by OSPAR as chemicals for priority action). All Member States (except SE) refer to the main sources of contamination (land-, sea- and air-based), with more details provided for land-based pollution. All Member States (except DK and PT) have directly referred to the results from the 2010 OSPAR QSR report (DK has made reference to the HELCOM HARMONY project) and a majority of countries have referred to the WFD monitoring methodology. There is a high level of coherence across the North East Atlantic marine region in the approaches used by the Member States to carry out the initial assessment of contamination by hazardous substances, radioactive substances and acute pollution events (although to a lesser extent for the latter). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States but one (FR) have made a judgement on the current level of contamination in their marine waters, but only two of them have made an assessment in relation to GES (IE, PT). The majority of Member States have made their disaggregated judgements in reference to the EQS or the EAC (except DK which has referred to HELCOM criteria).
+Only two Member States (DK and SE) have made an assessment of the impacts of contamination on seabed habitats while all Member States (except BE and PT) have assessed impacts on species.  Imposex is the biological effect most reported on but other biological effects (e.g. lysosomal membrane stability) have also been assessed. In the reporting sheets, only two Member States have provided a quantification of the proportion of seabed habitats impacted by contamination by hazardous substances (less than 1% for one Member State (UK) and 5-25% for the other (DE)). Only one Member State (UK) has made a quantitative assessment of the number of functional groups impacted by contaminants (1 group out of 30). 
+Only a few Member States (DE, ES, FR, IE) have made a judgement on the impacts on ecosystem components in relation to GES (i.e. the impact on ecosystem component is considered acceptable/not acceptable). 
+All Member States but one (PT) have made an assessment of contamination by radionuclides, most of them including a quantitative assessment (in particular of C-137) and description of main sources (BE, DE, ES, FR, IE, SE, UK). Most countries refer to OSPAR or HELCOM to state that concentrations are low and unlikely to have effects on ecosystem components.
+All Member States but one (PT) have made an assessment of contamination by acute pollution events but to a varying degree of detail. All countries but two (PT, SE) report on the number of oil spills or related events. In terms of impacts, only two countries refer to the OSPAR EcoQO on oiled guillemots (FR, NL). 
+In terms of data and knowledge gaps, very few Member States have reported substantially on this. The information gaps mentioned concern the need to develop assessment criteria to assess the impacts on ecosystem components and the difficulties to aggregate the different assessments to make a judgement in relation to GES. Gaps are also noted in terms of methodologies to make common assessments of radioactive contamination and contamination by oil pollution. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have set environmental targets for Descriptor 8. Countries with several marine subregions within the marine region have often defined targets per subregion (ES, FR) but with limited differences across the subregions. The UK has not made a distinction between the North Sea and Celtic Sea in the setting of its targets. Overall, the level of coherence in the setting of environmental targets and associated indicators for D8 across the North East Atlantic marine region is relatively high.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of targets, not counting associated indicators, varies from 1 (FR) to 11 (BE) with an average of four targets per Member State. The level of detail varies from one Member State to the other. Most Member States have set measurable targets because these are defined against specific reference levels (e.g. EQS, EAC) but no Member State has set threshold values and baselines for all its targets (although BE comes very close). 
+Most countries have set targets that are very close to their GES definition, using, as their main target, compliance with reference levels (whether the EQS or the EAC). Only few countries have directly specified the substances that should be measured (BE, DK).  
+Few Member States have defined pressure-reduction targets. Four Member States have set one or several targets on the reduction of contamination from land-based sources (DE, ES, FR, SE), three on contamination from air-based sources (DE, FR, SE) and only two on contamination from sea-based sources (DE, FR). In addition, two countries (IE, NL) have set a target for levels of contaminants to decrease (in addition to being below the reference levels) but without specifying which pressure should be acted upon for this to happen. 
+Most Member States have defined targets on biological effects of contaminants (except FR and PT). Most Member States have used OSPAR’s EcoQOs or EAC/ERLs as reference levels (BE, DE, DK, IE, NL, UK), including the OSPAR EcoQO on imposex (BE, DK, IE, NL) and the OSPAR EcoQO on oiled guillemots (BE, DE, NL). Some Member States have included other biological effects as indicators, e.g. cell damage, lysosomal stability, fish disease index (BE, DK, SE). Finally all Member States but one (PT) have set a target on acute pollution events, targeting illegal discharges and oil spills. Six Member States have used the common OSPAR target on the minimisation of acute pollution events and their impacts on biota or a similar target (BE, DK – except impact on biota, ES, IE, NL, UK). Only one Member State (DE) refers to the MARPOL Convention. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for Descriptor 9 for their entire marine waters, not distinguishing between subregions. Overall, the level of coherence in the definitions of GES for Descriptor 9 in the North East Atlantic marine region is high.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only three Member States (ES, FR, SE) have defined GES using the entirety of criterion 9.1 of the Commission Decision, i.e. including a criterion on the maximum frequency of regulatory levels being exceeded. The other Member States have defined GES only in accordance to the levels of concentration of contaminants. Almost all Member States refer to compliance with EU Regulation 1881/2006 and certain Member States also refer to its amendments (IE, NL, SE, UK). For two Member States (DK, PT), the reference is either indirect (in the accompanying text, mention of EU thresholds) or uncertain (reference to other EU standards indirectly related to Regulation 1881/2006). Two Member States (BE, FR) have included microbial pathogens in the scope of their GES definition (by including compliance to Directive 2006/113/EC as a criterion for the achievement of GES) and one (DE) has mentioned it in the accompanying text.
+Only two Member States include details about the specific substances that are covered in the GES definition (NL, SE). For the other Member States, the lack of specification seems to indicate that all relevant substances for fish and seafood in Regulation 1881/2006 are covered. Only one Member State is specific with regard to which species are covered by the GES definition (SE) while two (IE, UK) add a restriction to their GES definition (exclusion of migratory species for IE and exclusion of fish liver for UK). Only two Member States have defined aggregation rules to assess when GES is achieved (ES, PT). Finally, no Member State has added a specification regarding the origin of the fish/seafood covered by the GES definition.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have undertaken an initial assessment for D9. Most assessments related to fish and seafood are done in conjunction with the assessment of contamination of the environment and ecosystem components by hazardous substances (see previous section). Only one Member State (SE) mentions the discrepancy between regulatory levels for contaminants in the environment and for contaminants in foodstuffs (i.e. the latter being less strict). Overall, there is a relatively high level of coherence across the North East Atlantic marine region in the approaches used to assess the level of contamination of fish and seafood.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A large majority of Member States provide details regarding the substances assessed (BE, DE, ES, FR, IE, NL, PT, SE). For all but one (DK), the assessment covers both synthetic and non-synthetic substances. The substances assessed are generally the same as those assessed under D8, except less numerous (as not all are relevant for human consumption).  The same eight Member States also provide information regarding the species assessed. The most common species assessed is the mussel. Fish and shellfish species are also assessed but few Member States list the specific species used for the sampling. Only one Member State (ES) has made an assessment in cephalopods. 
+All but one Member State (BE) has made a quantitative assessment of the levels of concentration of contaminants in these various species. Out of these, all but one (PT) have assessed the current concentration levels against the levels specified in Regulation 1881/2006. However only two Member States (ES, UK) have provided, in the reporting sheets, a quantification of the proportion of fish and seafood samples tested, in which maximum levels have been exceeded and the results were very low in both cases (less than 1% of the samples). In a few cases, Member States have provided an aggregated judgement on the current levels of contamination in fish and seafood for human consumption: acceptable (i.e. status is good) for three Member States (ES, IE, NL), not acceptable (i.e. status is not good) for one Member State (DE). Other Member States (e.g. UK) have given an indication that the thresholds are rarely exceeded. One Member State (PT) has made an assessment using standards other than Regulation 1881/2006. 
+A majority of Member States have made an assessment of the levels of contamination of their shellfish and bathing waters, using as threshold values the standards of Directives 2006/113/EC (Shellfish Water Directive) and 2006/7/EC (Bathing Water Directive). 
+Finally, in terms of good practices, three Member States have assessed the current levels of radioactive substances in fish and seafood for human consumption (IE, NL, UK); only one Member State (UK) has discussed the issue of the origin of the samples used for the assessment.  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All but one Member State has set environmental targets for Descriptor 9. Sweden has not defined specific targets for D9 but states that its targets for D8 cover D9. Countries with several marine subregions within the marine region have often defined targets per subregion (FR, ES) but with limited differences across the subregions. The UK has not made a distinction between the North Sea and Celtic Sea in the setting of its targets. Overall, the level of coherence in the setting of environmental targets for D9 across the North East Atlantic marine region is very high.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two Member States (DE, ES) have defined more than one target but often only one is directly related to D9, while the other ones are more general, covering the various contaminant and eutrophication descriptors. 
+Half of the Member States have defined targets or indicators that relate to the reduction of a pressure (DE, ES, FR, NL, SE). These targets have often been defined for D8 and applied to D9 as they address the same sources of contamination. In addition to these pressure targets, all Member States (but SE) have defined an impact/state target, which requires concentration levels to comply with EU Regulation 1881/2006 on contaminants in foodstuffs. Sometimes the reference is explicit, sometimes it is indirect in expressions such as “national and international legislation” (NL), “Community legislation” (DK, ES), “EU limits” (DE), etc. Because of the systematic reference to the EU standards, all of these targets are considered to be measurable even when they are not detailed (i.e. there is no need to define specific threshold values and baselines). A few Member States (BE, DE, FR) have also included compliance with Directive 2006/113/EC on the quality of shellfish water to deal with microbial pathogens. 
+Only one Member State (DK) provides a detailed list of the substances covered by its environmental target while another (NL) gives details in the accompanying text. The lack of specification by the other Member States suggests that the substances covered are those of Regulation 1881/2006 which are relevant for fish. None of the Member States provide details of the specific species to be used for measurements, except one in the accompanying text (NL) and one which excludes a number of species, in line with its GES definition (IE). 
+Only two Member States include the issue of the origin of the samples in their environmental target, one indirectly by stating that the fish and seafood for human consumption falling within the scope of their MSFD target should come from their marine waters (IE) and one with a specific indicator on the traceability of the fish products (ES) (surprisingly, it is not the same Member State that included this aspect in its GES definition and that defined a target on the origin and traceability of samples). Only one Member State (NL) has defined an indicator relating to indicator 9.1.2 on the frequency of regulatory levels being exceeded. This is not surprising considering that this indicator was rarely used in the GES definition but surprisingly, none of the Member States that considered this aspect in their GES defined a specific target/indicator on this criterion. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States but one (FR) have reported the GES definition at the descriptor level without further elaboration. The GES definition in all Member States follows the descriptor definition in the 2010 Commission Decision. Overall, the level of coherence in the definitions of GES for Descriptor 10 in the North East Atlantic marine region is high. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">One Member State (FR) reported a GES definition up to the indicator level and provided details on how progress can be measured. Despite the lack of detail, some Member States provided additional elements to the GES definition that are not covered by the Decision. To achieve GES, the amount of marine litter should reduce over time in 7 out of 10 Member States (BE, ES, FR, IE, NL, SE, UK). One Member State (SE) furthermore reports that in the long term the marine environment should be free of litter. Three Member States (DE, DK, FR) refer to marine litter as a pathway for the proliferation of invasive NIS species. The same three Member States report that marine litter should not have adverse economic consequences for the maritime economic sectors (including shipping and fisheries) and coastal communities. Two Member States (FR, DE) further specify that marine litter should not have a risk for human health. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most Member States report on the lack of an agreed methodology and state that up to the reporting date, monitoring of marine litter is not systematically done. Efforts in the North East Atlantic Ocean to monitor marine litter have largely been done as part of international cooperation, under OSPAR and the International Bottom Trawl Survey (ITBS). Agreed OSPAR methodologies, commonly used and for which most data is reported, are related to beach litter monitoring and the analysis of plastics in the stomach of Fulmars. Data from fishing for litter projects are reported by three Member States (BE, NL, UK). Fishing for litter is the methodology to collect litter at sea by fishermen, and covered by OSPAR Recommendation 2010/19.  The overall level of coherence in the assessment of marine litter by the North East Atlantic Member States is high.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Little information is reported on the water column, including floating macro-litter and micro-particles. Better insights are also to be gained on the impact of marine litter on marine life and habitats. Only two Member States (ES, FR) report results on several species, including sea turtles, mammals and birds.
+In the reporting sheets, eight Member States (BE, DE, DK, ES, IE, NL, SE, UK) have reported on the input of marine litter on the shores, in the water and on the seabed, but each one using a different unit. The units used mostly express the ratio of the number of items or the weight (e.g. kg, tons) present on a certain surface area (e.g. km2, 100m beach). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The defined targets for marine litter are a good starting point for all Member States, but require further elaboration. For six out of 10 Member States, all targets are measurable. For two Member States (DE, FR), some targets are measurable while others are not. For two other Member States (IE, SE), none of the targets are measurable. One Member State (SE) however is ambitious and states that the marine environment, as far as possible, should be free from litter. The overall level of coherence in the setting of targets for marine litter across the North East Atlantic marine region is moderate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Targets aiming to reduce the amount of litter are defined by all Member States. Most Member States have defined 1-3 reduction targets. Four Member States defined more (3-6) reduction targets. All Member States but one (DK) intend to remove existing waste from the marine and coastal environment. Quantitative threshold values have not been set, except when the EcoQO target on the ingestion of plastic by Fulmars is cited (by two Member States only – BE and NL).
+Most Member States (except DE, DK, SE) have set a target to reduce visible litter from beaches. The second most-defined target is to reduce the impact on marine life (four Member States – BE, DK, IE, NL). Two Member States (NL, BE) cite the OSPAR EcoQO target on fulmars, while four Member States (DE, FR, IE, PT) indicate its potential use as indicator. In addition, one Member State (DE) has set targets to reduce the entanglement of birds with marine litter. Three Member States (DK, ES, UK) require more data and knowledge prior to setting an indicator on the impact of marine litter to marine life and habitats. As a consequence of the physical absence of Fulmars, the EcoQO target is not relevant for four Member States (ES, FR – Bay of Biscay only, PT, SE). 
+Targets that aim to reduce litter from the seabed and water column have only been set by two Member States. The use of aerial surveys to assess floating litter, as included in the targets of one Member State (ES), is considered a good practice. One Member State (BE) also set a target for 'fishing for litter'. One Member State (DK) intends to further research the potential use of fishing for litter data.
+Further good practices are the targets (by 5 Member States) set to reduce the entry into the marine environment of new waste from either land- or sea-based sources. Two Member States (DE, FR) aim to reduce the total entry of waste in the marine environment, while one (ES) focuses on the pathway of waste water discharge and other terrestrial sources. One Member State (DK) aims to reduce littering by beach tourists. One Member State (PT) confirms its commitment to the MARPOL Convention and the collection of shipping waste in the Directive on Port Reception Facilities.
+Targets to improve the knowledge base have been set by four Member States, covering the data and knowledge needs on the impact of marine litter on marine life and marine habitats, origin and dispersion of marine litter, litter at the seabed and micro-particles on the beach and in the water column.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for D11 but they have used different approaches. Two Member States (NL, PT) provided a definition of GES that is a copy (or very similar) to the D11 (and criteria and/or indicator) definition of the 2010 Commission Decision. Other Member States (FR, UK and to a certain extent SE) provided definitions which are in line with the definitions of the 2010 Commission Decision but are further developed. Another group of Member States (BE, DE, IE), for various reasons, are not (or only roughly) in line with the definitions of the 2010 Commission Decision. Finally, a last group of Member States (DK, ES) provided definitions of GES that appear to have been based on different interpretations (that could be considered as misinterpretations) of the 2010 Commission Decision. The level of coherence of the definitions of GES across the North East Atlantic marine region is considered to be low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Although most of the Member States defined GES at descriptor and criteria levels (with the exception of PT), a few of these Member States (BE, DK) did not (clearly) make use of both criteria of the 2010 Commission Decision. Only one Member State (DE) has covered other sources of energy in its definition of GES, namely, light, emission of electromagnetic fields and heat. Only three Member States (DE, FR, UK) have provided threshold values, meaning that the other definitions are all qualitative.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Half of the Member States undertaken very limited assessments (or did not carry out an assessment at all) on underwater noise (BE, DK, NL, PT, SE). The other half provided a more detailed assessment (DE, ES, FR, IE, UK). The level of coherence of the initial assessments on underwater noise across the North East Atlantic marine region is considered to be relatively high as the vast majority of the Member States (albeit with different levels of detail) focused on the identification of the sources of underwater noise, the acknowledgment of gaps and the need for future monitoring.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+In most cases, the initial assessment is very limited and general – one Member State (BE) has not made a distinction between impulsive and continuous sound – and does not go much beyond the identification of the main causes of pressure and the acknowledgment of information gaps. When information is provided in a more consistent matter, it is nonetheless in most cases descriptive and more focused on pressures than impacts. Only a few Member States (e.g. DE) try to quantify some parameters. In the reporting sheets, only two Member States have made a quantification of the proportion of their assessment area affected by the noise pressure but they are not based on the same criterion. One of them (FR) looks at continuous sounds and concludes that 75-100% of its area is affected while the other one (IE) looks at impulsive sounds and concludes that less than 1% is affected. No Member State has provided a clear conclusive judgement on the level of pressure or impacts.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States but two (IE, SE) have defined environmental targets and associated indicator for D11. The level of coherence in the setting of environmental targets (and indicators) for D11 across Member States of the North East Atlantic marine region is considered to be low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The response to D11 is very diverse in terms of setting targets. Two Member States have not defined any environmental targets for D11 (IE, SE) and another four Member States (ES, FR, NL, PT) have included high-level objectives that are not measurable rather than concrete targets. Two Member States (ES, PT) have also defined monitoring targets. Two Member States (BE, DE) have opted to define very concrete noise exposure criteria that are also applied in EIA regulation of wind farms, instead of defining pressure-based targets/indicators. One Member State (DK) reported only a target for impulsive sounds, but which is in line with indicator 11.1.1 of the 2010 Commission Decision. Finally, one Member State (UK) opted for very concrete targets that further develop the conceptual approach behind the indicators which are essentially pressure-based. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for Descriptor 1 however none of the seven Member States of the marine region have defined GES the same way (or even similarly). The levels of details vary enormously. This being said, all Member States but one (CY) have defined GES more specifically than in the text of Annex I of the MSFD and most Member States have incorporated some or all of the Commission Decision criteria for D1. One Member State has provided specific definitions for each criterion (FR) and five Member States have covered certain criteria but not all (ES, EL, IT, MT, SI). The coverage of the Commission Decision indicators is much less systematic with only two Member States covering all or most indicators but without necessarily all elements to make them measurable (ES, FR) and other Member States covering them only partially either explicitly (IT, MT) or implicitly in the criteria text (EL, SI). The level of coherence across the Mediterranean for the definition of Good Environmental Status for Descriptor 1 is low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For all Member States (EL, ES, FR, IT, MT, SI) except one (CY), the GES definition covers at least the species, habitats and ecosystem levels but to varying levels of details.
+With regard to the definition at species level, only one Member State addresses specifically the five main groups of highly mobile species – mammals, birds, fish, cephalopods and reptiles (ES). For the remaining five Member States, specific species groups are not explicitly mentioned (CY, EL, FR, IT, MT, SI). However, three Member States use the concept of “functional group” in their GES definition (ES, FR, SI). 
+In terms of specific species addressed in the GES definitions, one dominant approach is apparent. Three Member States (EL, ES, IT) in their GES definition state how attributes of specific species will be assessed in order to assess GES while one in their additional text has clarified which species will be used to assess GES (SI). 
+Three Member States (ES, IT, SI) refer specifically to the Birds Directive and one to the Habitats Directive (SI), thereby including listed species in the scope of their GES definition. In addition, one Member State mention listed/protected species (EL) but does not specify the legislation and/or agreement to which this mention refers. 
+With regard to the definitions at habitats level, only one Member State uses the concept of predominant habitats as defined for the purpose of the MSFD (FR). Four Member States out of six are not specific with regard to the habitat types covered by their GES definition (CY, EL, MT, SI), which would suggest that all habitat types are covered equally under the GES definition. One Member State refers to specific habitats in its GES definition (IT) and three Member States specifically mention Posidonia Oceanica (EL, ES, IT). 
+Only two of the Member States in the marine region make a direct mention to the Habitats Directive in their GES definitions (SI, ES). Another includes a specific mention to listed/protected habitats (EL) although the specific legislation and/or agreement to which this mention refers is not given. 
+With regard to the definitions at ecosystem level, a majority of Member States have defined GES so that it covers the whole ecosystem structure (EL, ES, FR, MT, SI). One of the Member States has set specific indicators for criterion 1.7, but this is only based on the condition of the birds and fish communities (ES). 
+In terms of baselines and threshold values, the approaches adopted by the Member States vary greatly. 
+Four of the Member States have used baselines in the sense of ‘reference conditions’, i.e. in relation to ‘prevailing physiographic, geographic and climatic (natural) conditions’ that are largely free from anthropogenic influences (CY, ES, FR, MT). 
+Half of the GES definitions for D1 in the Mediterranean region are qualitative (CY, FR, MT, SI). Three Member States have defined GES for specific species/habitats, using different thresholds for different features (EL, ES, IT) although not all thresholds are fully determined and quantified. Five Member States have integrated the principle of ‘reference condition plus acceptable deviation’ (EL, ES, FR, IT, MT). Finally, one Member State has included the notion of ‘restoration’ of biodiversity in their definitions (EL). 
+Two of the Member States have reflected in their GES, where appropriate, the definitions for Favourable Conservation Status under the Habitats Directive and for Good Ecological Status under the Water Framework Directive (ES, SI). In one case (ES), it relates to one specific habitat, Posidonia Oceanica, which should achieve both good ecological status (WFD) and favourable conservation status (HD). In the other case (SI), it is a general mention that favourable status as defined in the HBD and good status as defined in the WFD should be maintained as a condition to achieve GES.  One Member State has clearly stated that while it will tend towards the Favourable Conservation Status of the Habitats Directive for all habitats, its achievement for all habitats is not considered realistic in the timeframe of the MSFD (ES). 
+Finally, none of the Member States have included in their GES definitions a reference to relevant regional and/or international agreements.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have carried out an initial assessment on physical loss and physical damage. The level of coherence of the initial assessments on physical damage and loss across the Mediterranean Sea marine region is relatively high. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+All Member States in the Mediterranean Sea marine region have covered most types of physical loss and physical damage albeit at different levels of detail. Thus, while the information reported by some Member States is comprehensive (e.g. ES), in other cases the information is rather limited (e.g. EL). Likewise, all Member States have listed, and some described in good detail (e.g. ES), the main causes of pressure – the construction and maintenance of ports (physical loss) and trawling fisheries (physical damage) are always referred to. The impacts of physical loss and physical damages are also always covered but usually in much less detail than in the case of pressures. Two Member States refer explicitly to the Water Framework Directive reports (e.g. CY and SI). Only one Member State (CY) presented clear conclusive judgments on the level of pressure of physical loss and physical damage and their impacts; however, most Member States provided qualitative judgements (usually rather general) for at least some parameters.
+In the reporting sheets, only two Member States (CY, SI) provided the proportion of their assessment area (and of their seabed habitats) that is affected by physical loss and physical damage. One Member State (CY) reported less than 1% was affected by physical loss and physical damage, while the other (SI) reported that physical loss affected 5-25% of their assessment areas, and physical damage impacted 75-100%.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have carried out an initial assessment on biological features. All Member States have reported on habitats and species/functional groups, but only half of them addressed ecosystems (CY, EL, ES). The level of coherence of the initial assessments on biological features across the Mediterranean Sea marine region is considered as low. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitats
+While most Member States in the Mediterranean Sea marine region covered at least a good share of the relevant seabed habitat types, two of them did not cover, or covered in a very limited way, water column habitat types (EL, ES). All Member States used the MSFD classification of predominant habitats or an equivalent system (in particular EUNIS Level 2 classification), although in one case the correspondence is not entirely clear (IT). When assessing the habitat, all Member States reported on habitat distribution, extent and condition, as well as on the main causes of pressure, albeit with different levels of detail. Thus, while one Member State (ES) has reported extensively another one (EL) has provided only limited information mostly based on existing literature. Only two Member States (CY, SI) has provided a clear and conclusive judgement on the current status for all habitats. However, the remaining Member States provide judgements for at least some habitats/areas. The Habitats Directive is explicitly mentioned by five of the Member States (CY, ES, FR, MT, SI).
+In the reporting sheets, four Member States (CY, ES, MT and SI) reported on listed habitats from the Habitats Directive and three Member States (ES, IT and SI) reported on listed habitats from the Barcelona Convention. Five member States (CY, ES, FR, MT and SI) have reported using the MSFD predominant habitat type classification. The predominant habitat types which have been most reported are shallow rock (three Member States), littoral rock (three Member States), littoral sediment (three Member States) and shallow mixed sediment (three Member States). All predominant habitat types have been reported on by at least one Member State but no Member State covers the entire seabed completely in its assessment. 
+Species/functional groups 
+Half of the Member States used a mixed approach to report on species and functional groups. One Member State reported only on species groups (CY), and two Member States reported only on functional groups (IT, SI). 
+With regard to species groups, five Member States (CY, EL, ES, FR and MT) covered at least birds, fish and mammals. One Member State did not report on birds due to insufficient data (IT) and another indicated that birds were covered under the reporting obligations of the Birds Directive and that mammals were covered under the reporting obligations of the Habitats Directive (SI). In the reporting sheets, only three Member States (CY, ES, MT) reported on listed species from the Birds and Habitats Directive and three Member States (EL, IT, SI) reported on listed species from the Barcelona Convention. 
+With regard to functional groups, four Member States have reported on fish functional groups (FR, IT, MT, SI), and three Member States have reported on reptiles (turtles) (ES, FR, MT). Only one Member State (MT) has reported on birds at functional group level and none has reported on mammals at functional group level.
+For the majority of Member States, the assessment includes information on species abundance and condition. All Member States provided at least a qualitative/descriptive judgement of the current status of at least some of the species/functional groups reported. All but one Member State (EL) referred explicitly to the Habitats and Birds Directives (but not clear in FR). The pressures reported most often as the main pressures on species are biological disturbance (unspecified) and extraction of species (all species). 
+Ecosystems
+Only three Member State (CY, EL, ES) have reported on ecosystems. The three Member States provided a limited description of the ecosystem structure and its functioning and reported on the main pressures. One additional Member State (IT) has also reported on ecosystems at sub-regional level but the information, however, consists exclusively on the identification of knowledge gaps for each of the topics to cover (i.e. ecosystem structure, ecosystem productivity, etc.) and the plans to address them. No Member State has provided a conclusive judgment on the current status of its ecosystems but one Member State provided a descriptive judgement (ES).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the biodiversity descriptors, all Member States of the Mediterranean marine region have defined environmental targets, except CY and MT, which have not defined targets for Descriptor 4. Overall, the level of coherence in the setting of targets and indicators for biodiversity across the Mediterranean marine region is low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Half of the Member States (EL, IT, SI) has defined separate targets for the three descriptors. The other half has addressed the three descriptors through one set of targets, usually grouping them by ecosystem component (e.g. habitats, fish, birds, mammals, etc.) The classification followed is not coherent across the three countries however. The number of targets to cover the biodiversity descriptors varies from two (CY) to 24 (FR). For one Member State (IT) it is difficult to assess what constitutes a target and what is accompanying text so the actual number of targets is difficult to determine. In general, the Member States have defined a large number of targets and/or associated indicators. 
+The biodiversity targets represent a mix of state-, impact- and pressure-targets, with a domination of state- and impact-targets. State-targets relate mostly to maintaining or improving the condition of specific ecosystem components (e.g. fish community indices) and impact-targets focus on reducing impacts from certain pressures on ecosystem components (e.g. dolphin by-catch, impacts on the seabed). The pressures addressed are mainly those related to fishing activities and/or causing physical damage to the seafloor (including selective extraction of species, dredging, bottom trawling, by-catch, discards, etc.). Shipping activities, infrastructure construction and land-based polluting activities (e.g. industries) are also flagged as pressures on biodiversity that need to be reduced to achieve GES. Two Member States have not defined pressure-targets at all (CY, EL). One Member State (SI) has included the necessity to prevent “deterioration due to human activities” but has not defined specific targets/indicators geared towards reducing a specific pressure/level of activity. 
+The Member States have often addressed specific species and habitats that are considered either sensitive/threatened and in need of protection (e.g. listed species from the Habitats and Birds Directive or from the Barcelona Convention), that have a particular function/ role in the ecosystem (e.g. top predators, biogenic substrates, benthic communities), that are particular sensitive to certain pressures (e.g. by-catch, ship collision, dredging) or that are well-studied and monitored. Examples of such species and habitats commonly addressed by the targets of the Mediterranean countries include Posidonia oceanica seagrass meadows (CY, EL, FR, MT, SI) and the loggerhead sea turtle Caretta caretta (EL, IT, MT, SI).
+Most Member States have addressed the main three species groups in their targets: fish, birds, mammals. One Member State (CY) has focused only on fish, which can be explained by the fact that birds (as a group) and individual turtle and seal species are reported to be currently at GES in the initial assessment. Another Member State (IT) has not addressed birds, which is in line with the fact that it did not cover birds in its initial assessment and has not included birds in its GES definition. Within the coverage of fish functional groups, only three Member States (ES, IT, MT) have addressed elasmobranchs (sharks, skates, rays, etc.). A number of Member States (EL, ES, IT, MT, SI) have also addressed reptiles (and more specifically turtles). In terms of habitat types, all Member States address benthic habitats in a general manner or through the condition of the benthic community. In addition, a majority of Member States have addressed corals (EL, ES, FR, SI) and a majority have defined targets for plankton (hence also covering water column habitats) (CY, EL, MT, SI). All Member States have, directly or indirectly, defined targets for protected/listed habitats (either specific to one protected habitat or at a general level). 
+In terms of quantification, a minority of the Member States (CY, IT, SI) have defined thresholds and baselines for their targets and indicators and not for all their targets/indicators systematically. Two of these Member States (CY, SI) even refer to a number of multimetric indices to assess the status of benthic communities. A number of Member States have defined quantitative parameters but without providing threshold values that allow to measure the achievement of the target (e.g. ES, FR, MT).
+Most Member States (ES, FR, IT, MT, SI) have directly referred to EU agreements but only one Member State (SI) has referred to the Barcelona Convention. The standards most commonly referred to include the Habitats and Birds Directives, the Common Fisheries Policy and the Water Framework Directive.
+Despite a number of commonalities across Member States on certain elements, the approaches used for the setting of targets and indicators differ greatly, with some Member States defining specific and numerous targets, covering all elements addressed in the GES definition (ES, IT, MT, SI), while others remain limited in scope (CY) and/or general (EL, FR). A minority have set quantitative thresholds (CY, IT, SI) while more than half have remained qualitative (EL, ES, FR, MT), sometimes with a potential for quantification (EL, MT). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States but two (CY, MT) have defined GES for Descriptor 4. None of the Member States have made separate definitions for Descriptor 4 for their different sub-regions.  The level of coherence across the Mediterranean marine region for the definition of Good Environmental Status for Descriptor 4 is low. There is however coherence between half the Member States for criteria 4.2 and indicator 4.2.1 which all use the same method to assess the status of large fish. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">None of the five Member States of the Mediterranean marine region, which have defined GES for Descriptor 4, have done it the same way. A majority of Member States (ES, FR, SI) have defined GES for D4 at the level of the criteria, one has defined D4 at descriptor and indicator level (IT) and one Member State has not followed the Commission Decision at all (EL). Three of the five Member States that defined D4 have not defined GES for criterion 4.1 of the Commission Decision (EL, IT, SI).
+Some Member States have defined GES in such a way that it covers all food web components (i.e. from plankton to higher trophic levels) (EL, FR, ES) but also include mention of specific food web components in their GES definition. Most Member States (EL, ES, FR, IT) refer to ‘key’ or ‘main’ species or functional groups. Several Member States refer to large fish in their GES definition (EL only specific to large pelagic species, IT, FR, SI). None of the Member States have included specific species as indicators of change in their GES definition although one makes reference to specific types of ecosystem components (e.g. mammals, bony fishes, zooplankton, seagrasses) as well as one specific type of habitat, Posidonia meadows (IT). 
+Only two Member States (EL, ES) have included a reference to the pressures on food web components, both refer to the pressure of selective extraction and one to eutrophication (ES). 
+One of the Member States (SI) has defined its baseline as being in line with “natural conditions” and two (ES, IT) as being in line with “prevailing natural conditions.” Three Member States (ES, IT, SI) have indicated that they will use the same threshold for indicator 4.2.1 which requires the weight of large fish caught by research vessels that are above a threshold length “Lcut” to be above a percentage of the total weight “Wlim”. The specific thresholds will be defined in 2018. 
+A number of Member States (ES, IT) also refer to the “maintenance” for at least some of the criteria/indicators (e.g. of the productivity of key trophic groups) but it is not clear whether it is maintenance in relation to a current status. Two Member States (ES, FR) include energy transfers between trophic levels in their GES definition. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for Descriptor 6. None of the seven Member States of the marine region have defined GES the same way. The level of coherence across the Mediterranean marine region for the definition of Good Environmental Status for Descriptor 6 is low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The majority of Member States (CY, ES, FR, MT, SI) have defined GES for Descriptor 6 at criteria level. One has done so implicitly in the text at descriptor level (EL). Four Member States (ES, FR, MT, SI) have explicitly defined GES for both criteria 6.1 and 6.2. 
+In terms of indicators, a few Member States have included some of the Commission Decision indicators in the scope of their GES definitions and one Member State has defined GES only at the indicator level for indicator 6.1.2 (IT). All of the Member States refer to the reduction of physical pressures from human activities on the seabed, either directly or indirectly (through reference to impacts). Three of the Member States (FR, IT, SI) have included a quantitative indicator on the percentage of area occupied by biogenic substrate that can be acted upon by human pressures, one (IT) has set the threshold at 0% impacted and for two (FR, SI) the threshold is not yet specified. The same three Member States (FR, IT, SI) also have quantified indicators for non-biogenic habitat impacted by human pressures but none of them have set a threshold yet.
+Criterion 6.2 on the condition of the benthic community is hardly ever specified through indicators. Two Member States have indicated the assessment of GES will be based on multi-metric indices (CY, EL), one (CY) specifically refers to the WFD and good ecological status. The definitions for criterion 6.2 of the other Member States are generally vague despite the fact that the condition of the benthic community is one of the most studied and well-documented aspect of biodiversity across most of Europe, for which a number of WFD indicators could be used.  
+Only two of the Member States (CY, IT) have specified the substrate types covered by their GES definition. Three of the Member States (EL, ES, FR) refer to the habitats selected for D1. In all three cases, the D1 definition includes a general condition covering all habitats equally, which would suggest that the entire seabed is covered under D6.
+None of the Member States mention a baseline in their GES definition and none of the Member States use the WFD principle of ‘reference conditions plus acceptable deviation’. 
+Four of the Member States (CY, EL, ES, SI) mention the need to maintain the status and integrity of the seafloor habitats to ensure their functioning. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for Descriptor 2 for all their marine waters, not distinguishing between sub-regions. Overall, the level of coherence with regard to D2 is considered as low in the Mediterranean region.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The large majority of the Member States sharing Mediterranean Sea waters have defined GES in a rather vague way. One Member State (EL) simply reproduces verbatim the definition of Annex I. One Member State (SI) has reproduced albeit in a slightly less precise way the criteria set by the Commission Decision. Three Member States (CY, EL, MT) have set GES only at descriptor level, two (IT, SI) at criteria level, and two (ES, FR) at both descriptor and criteria level. None of the Mediterranean Member States have covered indicator 2.2.1, generally considered as too demanding in terms of monitoring.
+Minimum requirements (no further increase of NIS which have an adverse effect on the ecosystem) are reflected in only three Member States (ES, FR, IT) definitions and partly for another Member State (EL).
+Amongst the other Member States, there are major differences as to the level of details and focus. Several Member States explicitly take a risk-based approach, addressing primarily vectors and pathways (EL, to a lesser extent ES, MT and IT), while all Member States except one (MT) refer to impacts (CY, EL, ES, FR, IT, SI). Only one Member State (ES) considers one specific type of invasive NIS (macroalgae) in its definition. The GES definitions address NIS in general (SI) or only invasive NIS (MT, IT) or both (EL, ES, FR). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have carried out an initial assessment for D2.  The level of coherence in the assessments carried out by the Mediterranean Member States of the NIS pressure is considered as high. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The initial assessment for D2 is, as a rule, based on existing literature or, in certain cases, expert judgement. One Member State (SI) has carried out additional studies for the initial assessment of D2.
+All Member States have provided an inventory of NIS present in their marine waters. The main vectors and pathways are generally described. The assessment of impacts remains extremely limited. When the level of pressure is provided, it is in a qualitative way. Five Member States (CY, EL, MT, IT and SI) have indicated a trend in the level of pressure, albeit in a very general manner, and only three (CY, MT, SI) have made a judgement of the pressure albeit with a low level of confidence. On the whole, Member States describe in details knowledge and data gaps and, more rarely, plans to address them, often with limited details and in a rather non-committal way.
+One Member State (ES) has identified risk areas based on cumulative pressure.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For D2, almost all Member States have defined environmental targets and associated indicators for all their marine waters, not distinguishing between subregions. The only exception is Cyprus which has not set environmental targets for D2. In conclusion, the level of coherence is low across the Mediterranean region in terms of environmental targets and associated indicators.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of targets varies from 1 (EL, IT) to 4 (ES). Out of the six countries which have set environmental targets, four established surveillance-type targets relating to monitoring (SI, MT), inventory (EL) or a early warning system (IT) target. In addition, two Member States (ES, MT) have set a target in relation to research. The environmental targets other than the surveillance-type targets mentioned above are mostly pressure/impact targets. However, the targets rarely mentions specific vectors/pathways (ES, FR) or specific NIS (ES). The level of details varies greatly from one Member State to another. In general, the environmental targets have been assessed as not fully SMART, in most cases because they are not measurable or lack specification. 
+Three Member States have set targets relating to the reduction of new introductions, also mentioning spreading (ES, FR, SI). Three Member States specified which vectors/pathways should be addressed (ES, FR, IT). 
+The associated indicators also vary, with one Member State who has not set associated indicators (SI), two have set only one indicator associated to the one single target (EL, IT), two Member States (ES, MT) have set 3 indicators and one (FR) four indicators.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States with marine waters in the Mediterranean marine region have defined GES for Descriptor 3. However for two Member States (EL, IT) it is uncertain whether they have an official GES definition or the GES definition provided by these countries was only defined for the purpose of doing the initial assessment. Overall the coherence for the definition of GES for Descriptor 3 in the Mediterranean marine region is low. Three Member States in particular (ES, FR, MT) have defined their GES in ways that significantly deviate from the other countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of the Member States has defined GES at the descriptor level for Descriptor 3 (MT). One has defined GES at descriptor and criteria level (FR) and the other Member States have defined GES at criteria and indicator level. 
+For criterion 3.1, most Member States have used Fmsy, except one Member State (IT) which uses the proxy F0.1, however, the threshold used in relation to this indicator varies between Member States. Three Member States (EL, IT, SI) have also applied the indicator exploitation rate “E” and set the threshold at 0.4, which is appropriate for small pelagic species. Four Member States (CY, FR, IT, SI) have also used the secondary indicator catch/biomass ratio for criterion 3.1. 
+For criterion 3.2, most Member States (CY, ES, IT, SI) have used the primary indicator 3.2.1 SSB in relation to the reference point SSBmy but with different thresholds for the number of stocks which should be at or above the reference point. One member state (FR) has used Bmsy-trigger when defining indicator 3.2.1.  Most Member States also apply the secondary indicator 3.2.2 biomass indices (CY, FR, IT, SL). Two Member States in their GES definitions require all stocks to be within safe biological limits (FR, IT) although for one (IT) this threshold is preliminary and might therefore change. 
+All countries but two (EL, ES) have applied criterion 3.3 although in one case it is in the text at descriptor level (MT). Indicator 3.3.1 of the Commission Decision has been used by three Member States (FR, IT, SI) while indicator 3.3.3 has been used by two (FR, SI). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have carried out an initial assessment for D3. Overall, the level of coherence of the initial assessments of the fishing pressure by the Member States of the Mediterranean region is considered low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The reference points used to assess stocks in the sub-region as well as the stocks reported varied within the Mediterranean as well as within the sub-regions. Three Member States assessed stocks in relation to the Fmsy reference point (ES, EL, MT), one (IT) using F0.1 which is a proxy for the Fmsy reference point, one (FR) using Bmsy, one (CY) using Fpa and SSBpa and a final one (SI) using species abundance trends within the ecosystem. For small pelagic species, two countries (EL, IT).  have used the reference point E&lt;0.4 There was also a discrepancy in the types of stocks assessed with three Member States assessing both demersal and small pelagic species, one (MT) assessing demersal and small as well as large pelagic species, one Member State (FR) only assessing large pelagic species and one (CY) assessing only demersal stocks. 
+In the reporting sheets, five Member States (CY, EL, MT, IT, SI) have provided a quantitative assessment of the extent of their assessment areas affected by various types of fisheries. Two Member States (IT, SI) have reported that up to 75-100% of their assessment areas are affected by all types of commercial fishing fleet, one (MT) has reported 5-25% for each fleet reported on, another one (CY) has reported a similar figure for vessels longer than 12m using mobile and passive gears but then decreasing figures for other types of fishing fleets. Then one Member State (EL) has reported between 5-25% and 25-50% of its assessment areas as being affected by commercial extraction of fish and shellfish (depending on the type of vessels). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For D3, all Member States have defined environmental targets and associated indicators for all their marine waters, not distinguishing between sub-regions. Overall, the level of coherence of the targets defined by the Member States of the Mediterranean region is considered low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The targets for the Member States often remain quite vague. Within the marine region, half of the countries have opted for pressure targets prescribing the reduction of fishing effort by following management prescriptions originating from EU legislation (e.g. CFP) and/or following the advice from scientific bodies (ICES, GFCM, ICCAT) to achieve certain goals. There is very little use of state targets (e.g. requiring the SSB of stocks to be above SSBpa). Furthermore three countries have targets related to recreational fisheries (FR, IT, SI). Two member states have targets related to elasmobranchi (ES, IT).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for Descriptor 5 and all have covered the three criteria of the Commission Decision in their GES apart from one Member State (CY), whose GES definition does not seem to have taken into account any of the criteria. In relation to the inclusion of the Commission Decision indicators the situation is not homogenous. Only one Member State (FR) has clearly covered all the indicators, but in any case the majority of Member States covered most of the indicators. There are two indicators which are excluded more systematically than the others: indicator 5.1.2 (nutrient ratios) and 5.2.2 (water transparency). Many Member States have failed to include criteria covering both pelagic and seabed habitats. Three Member States (IT, ES, EL) focused only on pelagic parameters. Overall, the level of coherence in the Mediterranean marine region for the definition of GES for Descriptor 5 is moderate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States refer to the appropriate normative definitions of ecological status classifications of the Water Framework Directive (WFD) for coastal waters. However, while in some Member States (CY, EL, MT) the relation between the MSFD GES and the WFD GES is not entirely clear, others explicitly equate MSFD GES to the WFD GES. In the case of one Member State (IT), it is stated in their GES definition that for MSFD GES to be achieved, the WFD coastal water bodies must be at least of 'good quality' for the WFD biological quality element 'phytoplankton' (but not ‘phytobenthos’). Only one Member State (ES) mentions explicitly MED POL, while the OSPAR approach appears to have been followed by two Member States (FR, IT). Less than half of the Member States (ES, EL, SI) incorporated quantitative thresholds in their definition of GES. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States in the Mediterranean Sea marine region have carried out an initial assessment for Descriptor 5. Although all Member States have covered the relevant nutrients – nitrogen and phosphorus – some have not provided much information on organic matter (EL and ES). In some Member States the information on nutrient and organic loads is not complete as the breakdown of total loads into individual source-derived loads is usually limited (e.g. FR and SI). Assessments of nutrient loads from aquaculture are provided by a number Member States, but a number of Member States (e.g. SI and EL) do not appear to have considered atmospheric deposition of nitrogen, and the only consideration of atmospheric deposition (from IT) includes only loads from local large agglomerations. All Member States have provided concentrations of nutrients in the water, even though in the case of one Member State (FR) the information is limited. Concentrations of organic matter have been estimated by only few Member States (CY and EL). Overall, the level of coherence in the initial assessment of nutrient and organic matter enrichment is moderate in the Mediterranean Sea marine region.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The information provided on impacts is usually less complete than for pressures. Most Member States have assessed impacts on both seabed and pelagic habitats, with the exception of two (IT, ES). The majority of Member States (ES, FR, IT, MT and SI) do not address, or address in little detail, the impacts on macrophytobenthos. All countries but one (IT) have presented a judgement on trophic status pressure and/or impact trends even if not always per reference to GES (e.g. FR, MT); where made, judgements on both pressures and impacts often appear to be sound, based on the information provided.
+In the reporting sheets, only two Member States (CY, EL) have provided a quantification of the proportion of the water column and of the seabed habitats which is impacted by nutrient and organic matter enrichment – the figures vary between less than 1% and 1-5%.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Descriptor 5, all Member States in the Mediterranean Sea marine region have defined environmental targets and associated indicators for their marine waters, usually not distinguishing between subregions (although Italy has an additional target for the Adriatic Sea sub-region). Overall, the level of coherence in the setting of targets for Descriptor 5 across the Mediterranean marine region is moderate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amongst Mediterranean Member States, there is a mixture of state/impact- and pressure-based targets. Pressure reduction approaches are presented by three Member States (FR, EL, IT), while two Member States (CY, SI) present state/impact-based approaches. Only one Member State (ES) has set combined state/impact- and pressure-based targets to reduce nutrient loads to and nutrient concentrations within the marine environment (where concentrations are currently increasing), and to achieve or maintain WFD good or high ecological status in coastal waters. Finally one Member State (MT) has defined only a single monitoring target. The targets presented by most Member States of the Mediterranean region are usually specific and potentially measurable although it is not always possible to assess if they are achievable and realistic, namely, because clear quantitative thresholds are not always provided (IT and SI are exceptions).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for Descriptor 7. Practically all Member States have determined GES at a general level (only at descriptor level, or including criteria but without specifying scale, indicator, habitats species and ecosystems). Beyond this general determination, which is usually close to the Annex I MSFD definition of GES, only one Member State (FR) has specified the environment components to be taken into account and given a list of relevant parameters. Overall, the level of coherence in the definitions of GES for D7 across the Mediterranean marine region is moderate.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only one Member State (IT) has established a clear link to the Water Framework Directive (WFD) normative definitions of ecological status classifications for coastal waters, while another Member State (FR) refers explicitly to other existing regulatory regimes to be complied with (EIA and SEA). Two Member States (FR, SI) refer to a list of potentially impacted environmental components e.g. specific seabed habitats, oxygen levels or current velocity, linking D7 to D1, D4 and D6. Only one Member State (IT) incorporates a quantitative threshold in their definition of GES, but even in this case it is not clear how the threshold value was selected. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have carried out an initial assessment for Descriptor 7. Some countries have produced less detailed reports, focused only on some areas (coastal) and with missing elements such as impacts on specific environment components (CY, ES); this is often based on the hypothesis that present status is at GES, which is assumed but not clearly demonstrated (e.g. CY, ES). Some Member States (CY, IT) focused only on some parameters (usually temperature and salinity). The level of coherence of the initial assessments on hydrological process across the Mediterranean is moderate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plans to address the existing knowledge gap are provided by most Member States (FR, EL, IT, ES). Only two Member States (FR, IT) explicitly refer to WFD reports while on the other hand nearly all of them (but EL) focus on the coastal zones. When reported, the proportion of the assessment area reported as affected by hydrological processes varies significantly from less than 1% (CY, ES) to 75-100%  in one Member State (EL), however, in this specific case the high percentage is justified by the fact that changes due to climate change were also taken into account under D7. While most Member States have provided trends and/or judgements on the level of pressure of hydrological processes, only two Member States (FR, ES) provide clear conclusive judgements on the impacts. Even though two Member States (CY, EL) have also reported judgements on the impacts of permanent alterations of hydrographical conditions, those judgements do not seem sufficiently supported by the information provided.
+Marine acidification is expressly mentioned, even if in some cases briefly, by most Member States (CY, IT, FR, MT, SI). The proportion of the assessment area that is affected by marine acidification has been only reported, in the reporting sheets, by one Member State (SI), which indicates that less than 1 % of their assessment area is affected.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two Member States (CY, IT) have not defined environmental targets to address Descriptor 7. Overall, the level of coherence in the setting of environmental targets for D7 across the Mediterranean marine region is low. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most of the Member States (CY, EL, ES, FR) assume that their waters are currently at GES and have defined general environmental targets more related to the GES definition than to specific targets for D7 (e.g. FR, EL). Two Member States (ES, MT) on the other hand have focused on EIA and SEA for new projects. All Member States but one (MT) that reported targets have opted for impact-based targets but only two Member State (ES, MT) has also reported clearly pressure-based targets. No Member State has made a clear link to the WFD objectives or to assessments for D1, 4 and 6 or defined clear thresholds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States of the Mediterranean region have defined GES for Descriptor 8 at national or regional level, not distinguishing between sub-regions (although Italy has defined GES at the level of the subregion, the conditions to achieve GES are the same in all three subregions).  Taking into account the level of development of this descriptor, the level of coherence in the definitions of GES for D8 across the Mediterranean marine region is considered moderate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most Member States have defined GES in a specific way for the two criteria of the Commission Decision: concentration and effects of contaminants. Only one country (CY) has defined GES at descriptor level and does not cover both criteria of the Decision. Only two Member States (FR, MT) have defined GES for indicator 8.2.2 on acute pollution events. Only one Member State (FR) has included in its definition for effects of contaminants (indicator 8.2.1) a list of specific biological effects to be measured to achieve GES (although without threshold values). Two Member States (IT, ES) have referred to biological effects but without details as to which ones are included in the definition. Other Member States (EL, ES, SI) have defined indicator 8.2.1 in reference to compliance with OSPAR’s environmental assessment criteria (EAC), which unlike the EQS are developed in an integrated manner taking into account the contaminants’ concentrations and their biological effects. One Member State (MT) has not defined GES for biological effects (8.2.1). Two Member States (EL, IT) have included radionuclides (more specifically 137Cs but also 2010Po) in the scope of their GES definition. Four Member States (CY, ES, FR, SI) have added a condition that concentration of contaminants should not increase over time.
+Half of the countries (EL, FR, MT, SI) refer to the three possible matrices for measurement of contaminant concentrations (water, biota and sediment). One Member State (IT) mentions only water and biota, while another one (ES) uses only biota and sediment, referring to the accumulation of hydrophobe contaminants. Four Member States (EL, FR, IT, MT, SI) have, directly or indirectly, included compliance to the Environmental Quality Standards (EQS) Directive as a requirement to achieve GES. One Member State (CY) refers to “target levels” without further specification as to what these should be. The last Member State (ES) bases its GES definition on compliance with the OSPAR standards only. Overall, four Member States (EL, ES, FR, SI) have referred to the OSPAR standards in their GES definition. Two of these (FR, ES) also have waters in the OSPAR region but the other two do not. For one Member State out of these two (EL), the reference is only indirect as it has defined its own levels, taking into account the EQS and the EAC. For the other Member State (SI), the OSPAR EAC are used only for criterion 8.2 on effects of contaminants, while the EQS remain the standard for concentration levels. 
+Only three countries (EL, FR, MT) have been specific with regard to the substances covered by their GES definition: one covers all priority substances and additional ones (FR), while the other covers only a selection of priority substances (EL). For two other Member States (IT, SI), reference to the EQS may mean that all priority substances are covered but there is a lack of specification. For the last two Member States (CY, ES), it could be assumed that the substances included in the GES definition are those assessed in the initial assessment, considering the strong links between the two, but there is also a lack of specification. 
+Only two Member States have defined (different) aggregation rules (ES, IT) and one additional Member State (FR) states that they should be defined later, leaving open the question whether the “all in, all out” rule should apply to all the other Member States. 
+Finally, only one Member State (ES) has referred to UNEP/MAP (more particularly to MEDPOL’s Background Concentrations for certain substances) while four Member States (EL, ES, FR, SI) have referred to, or used, OSPAR’s Environmental Assessment Criteria and Background Criteria.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have carried out an initial assessment for D8. There is a moderate level of coherence across the Mediterranean marine region in the approaches used by the Member States to carry out the initial assessment of contamination by hazardous substances.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only three Member States (ES, FR, MT) have provided a detailed, quantitative, assessment of the level of contamination. The remaining Member States have either provided dated or incomplete information (CY, EL) or made a very limited assessment covering only some parameters (IT, SI). Practically all Member States (not IT and SI) have provided a list of the contaminants considered in their assessment. The most common man-made substances assessed include PCBs and PAHs and the most common heavy metals assessed include cadmium, lead and mercury. All Member States refer to the main sources of contamination (land-, sea- and air-based), albeit with very different levels of detail. In any case, the information on land-based pollution is systematically more detailed. Half of the Member States referred directly to the WFD monitoring (CY, ES, FR, MT) and only three Member States refer explicitly to the Barcelona Convention or MED POL (CY, ES, MT). Only two Member States (ES, MT) refers explicitly to the EQS.
+Only two Member States (CY, EL) have made an assessment on the impacts of contamination on seabed habitats while all Member States except two (ES, IT) have assessed impacts on functional groups. In the reporting sheets, no Member State has provided a quantification of the proportion of seabed habitats impacted by contamination by hazardous substances. 
+All Member States but two (IT, FR) have made a judgment on the current level of contamination in their marine waters. Three Member States (EL, ES, FR) have made a judgment on the impacts on ecosystem components. 
+All Member States but two (MT, SI) have made an assessment of contamination by radionuclides, most of them including a quantitative assessment (in particular of C-137) and description of main sources (CY, EL, ES, FR). All Member States but one (IT) have made an assessment of contamination by acute pollution events but to a varying degree of detail. All countries but two (CY, IT) reported on the number of oil spills or related events. 
+Only two Member States (EL, ES) have provided a fair amount of information on data and knowledge gaps and described in detail the plans to address them.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have set environmental targets for Descriptor 8. Overall, the level of coherence in the setting of targets for D8 in the Mediterranean marine region is low. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of targets, not counting associated indicators, varies from 1 (CY, EL) to 13 (FR). The level of detail in the targets varies from one Member State to another. Most Member States have set measurable targets because these are defined against specific reference levels (e.g. EQS, EAC) but they are often rather an expression of GES than targets defined to help achieve GES. 
+One Member State (FR) has defined pressure-targets, which are geared towards reducing input of contaminants to the sea from land-, sea- and air-based sources. Four Member States (CY, IT, MT, SI) have defined state-targets, i.e. targets that are solely geared towards the non-exceedance of reference levels. One Member State (ES) has used a mixed approach, defining both pressure- and state-targets and one Member State (EL) has defined only a monitoring target, which requires to investigate and determine concentration levels. The reference levels used in the targets of five Member States are those of the EQSD/WFD and/or of OSPAR. Only two Member States (CY, MT) have specified the contaminants that should be measured but for two other Member States (IT, SI), it can be inferred that the contaminants to be measured are those covered in the EQS Directive. Only one Member State (SI) has defined targets for radionuclides (in line with its GES definition).
+Less than half of the Member States (ES, IT, SI) have defined one or several targets focused on indicator 8.2.1 on biological effects. The targets are relatively general, only one Member State (ES) refers to internationally-agreed criteria for biological effects. Only three Member States (ES, FR, MT) have defined one or several targets on indicator 8.2.2 on acute pollution events (which is in line with the fact that only one Member State has defined GES for acute pollution events). One (ES) uses the OSPAR-agreed target, one (FR) has defined seven pressure-targets to reduce discharges of hydrocarbons and other pollutants from ships and their impacts and the last one (MT) has defined a data collection target. Only one Member State (FR) refers to regional/bilateral cooperation in the Mediterranean region in its targets. 
+Finally, three Member States (ES, MT, SI) have defined monitoring/knowledge targets in addition to pressure- or state-targets, which are geared towards collecting more information on a certain number of gaps, in particular biological effects/biomarkers.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States have defined GES for Descriptor 9. Overall, the level of coherence in the definitions of GES for Descriptor 9 in the Mediterranean marine region is high.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only two Member States (ES, FR) have defined GES using the entirety of criterion 9.1 of the Commission Decision, i.e. including a criterion on the maximum frequency of regulatory levels being exceeded. The other five Member States have defined GES only in accordance to the levels of concentration of contaminants. Almost all Member States refer to compliance with EU Regulation 1881/2006 but none directly refer to its amendments. For one Member State (CY), the reference is indirect (reference to Community legislation in the definition which is assumed to mean Regulation 1881/2006). Only one Member State (FR) has included microbial pathogens in the scope of its GES definition (by including compliance to Directive 2006/113/EC as a criterion for the achievement of GES).
+Only one Member State (EL) has included details about the specific substances that are covered in the GES definition. For the other Member States, the lack of specification seems to indicate that all relevant substances for fish and seafood in Regulation 1881/2006 are covered. The same Member State is also the only one to be specific with regard to which species are covered by the GES definition. The other Member States remain vague, referring to fish, fishery products, shellfish, molluscs, etc. but without further specification. Only two Member States (ES, IT) have defined (similar) aggregation rules to assess when GES is achieved. Finally, a number of Member States (IT, SI, EL) have included a mention about the origin (from national waters) of the samples to be used to assess whether GES is achieved.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States but one (IT) have carried out an initial assessment for Descriptor 9. Overall, there is a moderate level of coherence across the Mediterranean marine region in the approaches used to assess the level of contamination of fish and seafood, including contamination by microbial pathogens.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most assessments related to fish and seafood for human consumption are done in conjunction with the assessment of contamination of the environment and ecosystem components by hazardous substances (see previous section). All of the Member States that have reported on contamination of fish and seafood provide details regarding the substances concerned. For all but two (CY, MT), the assessment covers both synthetic and non-synthetic substances. The substances assessed are generally the same as those assessed under Descriptor 8, except less numerous (as not all are relevant for human consumption). All of the Member States that have reported also provide information regarding the species or the functional groups used for the assessment but, for many Member States, the information remains general (individual species not named). In terms of individual species, the most common species assessed are the Mediterranean mussel and the red mullet. Less than half of the Member States (ES, FR, IT) have made an assessment in cephalopods. 
+All Member States have made a quantitative assessment of the levels of concentration of contaminants in these various species against the levels specified in Regulation 1881/2006. Most Member States (e.g. CY, EL, MT, SI) have given an indication that the thresholds are rarely exceeded. Only two Member States (CY, EL) provide a clear aggregated judgement on the current situation in relation to GES.
+In terms of good practices, one Member State has assessed the current levels of radioactive substances in fish and seafood for human consumption (EL); an additional Member State (CY) has provided a judgement on the level of impact but it is not clear how it reached that conclusion.  
+All Member States provided information on microbial pathogens, making an assessment of the levels of contamination of bathing waters referring to Directive 2006/7/EC (Bathing Water Directive). All but three Member States (CY, MT, SI) assessed the levels of contamination in shellfish waters referring to Directive 2006/113/EC (Shellfish Water Directive). Only three Member States (CY, EL, MT) provided a conclusive judgment on the status of their waters, which was considered “good” in all cases.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Four out of seven Member States (CY, EL, ES, SI) have set environmental targets for Descriptor 9. Overall, the level of coherence in the setting of environmental targets for D9 across the Mediterranean marine region is high.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of targets defined to cover D9 vary from one (CY, EL) to four (ES). Most Member States have also defined associated indicators, which provide the parameter that should be measured to assess the achievement of the target. In general, all Member States that have defined targets for D9 have set one target related to the non-exceedance of regulatory levels as defined in Regulation 1881/2006. One Member State (CY) has allowed deviation from “reference levels” (which is understood to mean Regulation 1881/2006). 
+None of the Member States that have defined targets for D9 have provided a list of the substances to be measured or the species to be used for measurement. The lack of specification suggests that the substances covered are those of Regulation 1881/2006 which are relevant for fish.
+Two Member States (ES, SI) have defined targets that are not only about compliance to regulatory levels. One Member State (SI) has defined a target related to the number of inspections of landed catch by fishing vessels. Unfortunately the target is not specific as the threshold value has not yet been determined by the country. The other Member State has defined two targets related to the reduction of contamination from land- and sea-based sources, which are the same targets as for D8, and one target relating to gathering more information on the traceability of fisheries product and the origin of the samples used to assess compliance with regulatory level and the achievement of GES. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GES for Descriptor 10 has been defined by all Member States that have reported in the Mediterranean marine region. Overall, the level of coherence in the definitions of GES for Descriptor 10 for the Mediterranean region is moderate. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only one Member State (FR) reported a GES definition that was assessed as adequate, up to the indicator level while providing details on how progress can be measured. All other Member States have defined GES at descriptor level without further elaboration. The GES definitions in all Member States except one (MT) are in line with the descriptor definition in the 2010 Commission Decision, but not with the definition of the indicators and criteria. Despite the lack of detail, some Member States added elements to the GES definition that are not covered by the Decision. To achieve GES, the amount of litter should reduce over time in all Member States except one (CY) although in one case this only refers to the input of litter (MT). One Member State (EL) furthermore aims in the long term to have litter-free coasts and seas. Two Member States (FR, SI) report that marine litter should not have adverse economic consequences for the maritime economic sectors and coastal communities. One Member State (FR) also refers to marine litter as a pathway for the proliferation of invasive non-indigenous species.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The reporting on the initial assessment of marine litter is assessed as adequate for all Member States, except one (CY).  Overall, the level of coherence in the initial assessment for Descriptor 10 for the Mediterranean region is moderate. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substantial data is reported on seabed litter by all Member States except two (CY and SI), detailing mostly the geographical distribution, densities, types of marine litter and in some cases also seasonal differences. Data is also reported on beach litter by all Member States but one (CY), often as a by-result of beach cleaning actions. Three Member States (FR, IT, SI) reported on micro-particles. Only one Member State (IT) has reported on micro-particles for the Western Mediterranean subregion. Two Member States (ES, FR) have also reported on floating litter. The impact of marine litter on biota is reported by five Member States (ES, FR, IT, MT, SI). Two Member States of the Adriatic Sea subregion (IT and SI) focused on the loggerhead turtle Caretta caretta as the indicator species, while two Member States of the Western Mediterranean subregion (ES and FR) analysed various species, including sea turtles, whales and dolphins. 
+Data has been reported for all subregions of the Mediterranean. Yet, for some subdivisions, data was not available, i.e. Levantine Sea (EL), South Adriatic Sea (IT) and the South Tyrrhenian Sea (IT).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States, except one (CY) have set targets for marine litter. One Member State (MT) has set a very basic knowledge target. Four Member States (ES, FR, IT, SI) have set measurable targets, including a target intending to remove existing waste from the marine coastline and the seabed. Targets on micro-plastics have been explicitly included by two Member States, one on water surface (IT) and one on water surface and seabed (SI). One Member State (FR) has set a target for more research on micro-particles.  No Member State has defined threshold values. The overall level of coherence in the setting of targets for marine litter in the Mediterranean Region is moderate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Targets that address the impact of marine litter on biota have only been set by one Member State (IT), which aims to reduce the volume and weight of marine litter found in the stomach or faecal pellets of sea turtles (Caretta caretta). The assessment is a promising alternative for the Fulmars target in the North-East Atlantic Ocean. Two Member States (ES, SI) require further research on the impact of marine litter on biota. Further good practice are the targets set by two Member States (FR, ES) to reduce the entry of new waste from land- and sea-based sources into the marine environment. One Member State (IT) has specifically set a target on ‘fishing for litter’, as an alternative to collect waste from the seabed. One Member State (ES) intends to gain a better understanding on the source and dispersion of marine litter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States that have reported have defined GES for Descriptor 11. The level of coherence in the GES definitions for D11 in the Mediterranean Sea is moderate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only one Member State (FR) has reported an elaborate GES definition, which states that GES is achieved when the abundance, mortality risk and communication behaviour of sensitive species is not affected by underwater noise. Even though limited detail is given and the GES definitions are unspecific, all Member States but one (MT) have included the sound types covered by the 2010 Commission, i.e. ‘loud, low and mid frequency impulsive sounds’ and ‘continuous low frequency sound’. In addition, three Member States (ES, FR, SI) have extended the scope of the GES definition in the Decision substantially and added high frequency impulsive sounds (e.g. originating from the sonar of pleasure boats) to their GES definition. No Member State has set thresholds values and reference values, but considering the limited data availability for D11, this can be expected at this stage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The level of information reported in the initial assessment for Descriptor 11 varies substantially. The initial assessments of three Member States (ES, FR, SI) are assessed as adequate. Three Member States (CY, EL, MT) have provided limited information, while one Member State (IT) has not done the initial assessment. The level of coherence of initial assessment for D11 in the Mediterranean Sea is low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most Member States give a qualitative review of the sources of underwater noise, being shipping, offshore exploration and production, port operations and defence.  One Member State (SI) reports on noise monitoring. Two Member States (ES, FR) have developed an inventory of the level of underwater sound, based on the sources than can produce underwater sound and visualised the results on a map. One of these two Member State (ES) reports the cumulative sound pressures, while the other (FR) has developed a separate map for ambient and impulsive sound. One Member State (SI) has done substantial, recent monitoring of underwater noise. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States except two (CY, IT) have reported at least one target on underwater noise. The targets of all Member States are unspecific and not measurable and mostly similar to the GES definition. One Member State (FR) made a specific reference to limit the acoustic disturbances to mammals and bird nesting sites. The level of coherence of the targets for D11 in the Mediterranean Sea is low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Member States except two (CY, IT) have reported at least one target on underwater noise. The targets of all Member States are unspecific and not measurable and mostly similar to the GES definition. One Member State (FR) made a specific reference to limit the acoustic disturbances to mammals and bird nesting sites. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None of the two Member States in the Black Sea marine region have defined GES for all three biodiversity descriptors (D1, D4, D6). Bulgaria has defined GES for both Descriptor 1 and Descriptor 6 in a single definition, while Romania has only defined GES for Descriptor 1. Coherence has therefore only been assessed for Descriptor 1. 
+One Member State (BG) has defined GES both at descriptor and indicator level while the other (RO) has defined GES only at indicator level. The two countries have followed different approaches with one Member State (BG) covering all habitats and species, while the other (RO) covers specific seabed habitats and associated communities, specific benthic species and one cetacean species. 
+The coherence between the GES definition of the two Member States of the Black Sea marine region is low. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitats
+The specific seabed habitats covered by the first Member State (RO) correspond to habitat types from the Habitats Directive. These habitats might also be covered in the other Member State’s GES definition through the reference that special habitats designated as endangered or vulnerable, including those under the Habitats Directive, should be effectively preserved by appropriate national and regional mechanisms. The second Member State (BG) effectively covers all seabed habitats and associated communities in its definition (except deep-sea coastal slope and abyssal plain, which it explicitly excludes from the scope of the GES definition) while the first one restricts to specific, already protected, habitats. However this Member State (RO) also uses the Ecological Evaluation Index (EEI) from the WFD as an indicator for the condition of macroalgae communities, hereby increasing slightly its coverage of seabed habitats. The two Member States cover Commission Decision criteria 1.4, 1.5 and 1.6 but only partially for selected habitats for the first Member State (RO). 
+Species
+In terms of coverage of species, one Member State (RO) covers only a few shellfish species and one species of cetaceans (the harbour porpoise). The other Member State (BG) covers fish and mammals (in general), defining a number of GES indicators for the distribution, abundance and condition of the species populations. It covers criteria 1.1, 1.2 and 1.3 of the Commission Decision but only for fish and mammals. It does not provide an indication of the exact fish and mammal species that are covered so presumably all species present in its marine waters are covered by the definition. 
+This Member State (BG) requires that good status under the WFD and favourable conservation status as per the Habitats Directive are achieved for fish species. It also covers “rare and endangered” fish and mammal species as per the appropriate legislation and international convention. Although not specified this may include the Habitats Directive, the BSC list of protected species and the ACCOBAMS agreement. The other Member State (RO) does not mention the Habitats Directive or the Black Sea Convention for protected/listed species. 
+Neither Member State has covered seabirds or cephalopods in their GES definition. 
+Ecosystems
+Neither Member State has defined GES for criterion 1.7 of the Commission Decision on the ecosystem structure. 
+In terms of baselines, one Member State (BG) uses the baseline in the sense of “reference conditions”, i.e. in relation to natural physical, geographical and climatic conditions, adding a condition to account for the sustainable use of the marine environment. The other Member State (RO) uses different baselines and thresholds, sometimes referring to an “historical” state but most of the time using the present state as the baseline.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One Member State (BG) has undertaken an initial assessment on both physical loss and physical damage; the other Member State (RO) has only provided information on physical damage. The assessments vary significantly in the level of detail provided with one Member State presenting a very limited assessment (RO) and the other (BG) presenting a more comprehensive assessment. The level of coherence in the approaches used for the initial assessments of physical damage and loss between the Member States is moderate the level of detail provided in the reporting varies quite a lot.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the reporting sheets, both countries have identified dredging, coastal works and ports as the main pressures causing physical damage. One Member State (BG) has also identified fisheries as a major cause of physical damage on their Northern and central shelf. 
+In the reporting sheets, both Member States have provided indications of the extent of the seabed impacted by physical damage. One Member State (RO) indicates that 5-25% is impacted while the other (BG) provides varying estimates for different regions ranging from 1-5% to 25-50%. One Member State (BG) has also provided estimates for physical loss which, depending on the area, range from 1-5% to 50-75%. 
+One Member State (RO) has not provided a judgement on the level of pressure from physical loss or damage but provides trends in the level of pressure from physical damage; the other Member State (BG) has provided a judgement on the level of pressure from physical damage for most areas (good in coastal areas, not good in shelf areas). In one Member State the level of pressure from physical damage is indicated as stable (RO) and in one as declining for all areas (BG). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The level of coherence of the initial assessments on biological features between the two Black Sea countries is considered as low. One Member State (BG) has reported on habitats within their whole marine region while the other (RO) has only provided information for their Natura 2000 sites. The approach to reporting on fish is done in relation to Fmsy by one Member State (RO) and using biodiversity indices for the other (BG). One country (BG) acknowledges a lack of sufficient information to assess the ecosystem while the other provided some information on specific ecosystem components. Both countries reported on the same marine mammal species. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitats
+Both Member States have reported on habitats in their reporting sheets, one (BG) has done so by reporting according to the MSFD predominant habitat types while the other (RO) has reported on three habitat types covered under the Habitats Directive and also provides information on specific habitat-forming species. Both countries provide more information in their paper reports, one has focused on the state of their Natura 2000 sites (RO) while the other (BG) provides more extensive reporting on the MSFD predominant habitat types but also refers to the Habitats Directive. The latter provides an overview showing how the habitat types listed in Annex I of the Habitats Directive, as well as several of their national subtypes, correspond to the predominant habitat categories of the MSFD (32 biotopes reported but indicated that this list is not yet complete). . 
+When assessing habitats or habitat types, both Member States have provided trends for habitat distribution, extent and condition; one Member State (RO) has also provided judgements on the status for habitat extent and condition (good). The trends provided by one Member State (BG) for all benthic habitats are indicated as declining while for the other (RO) they are indicated as stable. 
+One Member State (BG) has reported on water column habitats in their reporting sheets while both Member States have reported information relevant to water column habitats in their paper report. 
+Species/functional groups 
+Both Member States have reported on species and functional groups but in both cases the reporting is limited to fish and cetaceans and certain habitat-forming benthic species. Both countries have reported on the following cetacean species: Tursiops truncatus, Delphinus delphis and Phocoena phocoena. The information for each of these species is limited as there is no targeted monitoring in one Member State (BG) while the other (RO) states that the monitoring is not structured according to MSFD standards. 
+In the case of fish, one Member State (RO) has provided fisheries data assessing how specific stocks, as well as demersal and pelagic stocks as a group, are exploited in relation to Fmsy. The other Member State (BG) uses the Bray–Curtis dissimilarity method to assess the group condition of demersal and pelagic fish and the Shannon-weaver and Simpson diversity indexes to assess the groups’ relative abundances; this Member State has not assessed specific fish species. 
+Ecosystems
+Only one Member State (RO) has reported on ecosystems in the reporting sheets and provides information the ecosystem structure and abundances of certain specific habitat types or habitat forming species at specific depth ranges but not a comprehensive ecosystem assessment. The other Member State (BG) has acknowledged the lack of information from the period of 2006 to 2011 and instead provides a general description of the characteristics of the Black Sea based on existing literature and focused on food chains. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have defined environmental targets for the biodiversity descriptors. One Member State (BG) has defined separated targets for species, littoral habitats, shelf habitats, shallow habitats and water column habitats while the other one (RO) has defined a number of habitats and species targets for specific areas.  The level of coherence in the setting of targets between the two Member States is low to moderate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have defined state-based targets but one Member State (BG) has also defined a number of pressure targets, focusing on the main pressures on the seafloor (e.g. fisheries, bottom-trawling, dredging, etc.)
+Both countries have defined targets dealing with fish, mammals and a range of habitats but none have defined targets for birds and cephalopods, in line with their GES definitions. The approach of one Member State (RO) is focused on specific species and habitats. The other Member State (BG) has defined targets covering on the one hand all fish and mammal species and on the other hand specific community-associated habitats. Therefore the targets formulated by this latter Member State (BG) cover a more comprehensive range of biodiversity components.
+The habitats covered in the targets of the two Member States are for the most part already protected under the Habitats Directive, in line with the GES definition. 
+The two Member States share targets for Donacilla Cornea, Pholas Dactylus, Donax truncules, Cystoseira Barbata and Mytillus Galloprovincialis. Most targets of both countries are SMART.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have defined GES. One Member State (BG) has defined GES at indicator level. In conclusion, the coherence between the GES definition of the two Member States of the Black Sea marine region is low. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of the definitions (in the paper report) aims at maintaining the low values of biomass and reducing the blooms and range of distribution of one specific species (M.leidyi), while the other one relates to the ratio between native species and NIS and the prevention of new introductions. 
+The other Member State (RO) has defined GES at criteria level. However, the definitions are not clear. The first one sets as an objective to prevent NIS from becoming invasive, while the second relates to environmental impacts of invasive NIS and remains very general.
+Both Member States refer to gaps in knowledge but only one (BG) details to a certain extent these gaps.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have carried out an initial assessment for D2. The level of coherence between the two Member States is considered high. Both Member States have paid particular attention to Mnemiopsis leidyi. Both Member States have also identified shipping as the main pathway of NIS introductions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have provided an inventory of NIS present in their marine waters. The main pathway identified by both countries is shipping. Both countries have identified Mya arenaria, Anadara inaequivalvis, Doridella obscura, Callinectes sapidus, Palaemon macrodactylus, Mnemiopsis leidyi, Oithona brevicornis as NIS in their marine waters. Some of the species reported by Romania have not been reported by Bulgaria and vice versa. Both Member States report in detail on Mnemiopsis leidyi.
+One Member State (RO) has reported that the level of pressure from NIS remains stable and the level of pressure is considered as acceptable (status is “good”). The other Member State (BG) has made no such judgements. One Member State (RO) states that further research is needed to assess impacts while the other (RO) states that more research is needed to make a judgement on the current level of pressure. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One Member State (RO) has not set environmental targets for Descriptor 2, which means that it is not possible to compare the two Member States’ approaches and therefore not possible to make an assessment of coherence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have defined GES for Descriptor 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One Member State (BG) has defined GES following the structure of the Commission Decision, applying both primary and secondary indicators for criteria 3.1 and 3.2 and a general statement for criterion 3.3. 
+The other Member State (RO) has not followed the Commission Decision and has applied what appears to be a target for a single stock. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The extent and detail provided in the initial assessments vary strongly between the two Member States, with one providing an extensive assessment (BG) while the other’s (RO) is extremely limited. The level of coherence of the initial assessments by the two Member States is considered as low. One Member State (BG) has provided a comprehensive picture of the situation of their fisheries while the assessment of the other Member State (RO) is very limited. Both countries however report on the same fish species.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both assessments indicate a situation of stocks being exploited at levels higher than Fmsy. An exception is sprat which is indicated as being exploited below Fmsy by one Member State (RO) but above Fmsy by another (BG). Both countries have reported on sprat, turbot, anchovy and whiting. One country (BG) also mentions cod in their assessment but does not do so in relation to stock assessment reference points. 
+Only one of the two Member States (BG) has reported on their fishing fleet and has done so extensively. The impacts on the environment that each of the Member States has reported on are different: one has reported more on seabed habitats (BG) and one on the effects on cetaceans (RO). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have set targets for Descriptor 3. One Member State (BG) has set 15 targets and the other (RO) 5 targets. All targets from the two Member States are stock-specific. The level of coherence is therefore considered low to moderate.  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In addition, in its paper report, one Member State (RO) has also set a number of targets relating to the improvement of fisheries in the Black Sea in general. 
+The targets of one Member State (RO), as reported in the reporting sheets, specify the necessary reduction in fishing effort needed by percentages, but are not clear as to how they relate to MSY or PA reference points. The other Member State (BG) has set targets that do relate to reducing fishing mortality to below Fmsy and additional targets to increase the SSB of certain stocks, to maintain the biomass of certain species above a certain level and the application of a number of length-based targets. 
+Both Member States have targets for sprat, turbot and anchovy. One Member State (RO) has also set targets for whiting and dogfish. The other Member State (BG) has reported that due to a lack of information they were unable to set targets for dogfish as well as Mediterranean horse mackerel, red mullet and the veined rapa whelk shellfish. 
+The approaches of the two Member States to setting targets are different although they cover three of the same species and both will require reductions in fishing mortality. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have defined GES for Descriptor 5, one (RO) at indicator level and the other (BG) at criteria level but integrating a number of indicators from the Commission Decision. It should however be noted that one of the Member States (RO) has phrased its GES definition in a way that seems to indicate that it is only a proposal and not a final, adopted, GES definition. Also both Member States have reported GES definitions in the reporting sheets which do not match their GES as defined in their paper reports. The level of coherence between the two Member States is moderate considering the uncertainties related to the lack of quantitative threshold values for a number of indicators. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The GES definitions as provided in the paper reports of the two Member States show many similarities. One Member State (RO) states that nutrient concentrations should decrease near pollution sources close to land while the other one (BG) states that nutrients should decrease in the coastal area. This Member State (BG) however also states that nitrogen should decrease in the shelf area while the other Member State (RO) requires nutrient concentrations in the water column and offshore waters to be maintained. 
+Both Member States have also defined GES for chlorophyll-a levels, which should be reduced in one Member State’s waters (RO) and be comparable to levels found where no anthropogenic pressure is present in the other Member State’s waters (BG). While not directly comparable, these two objectives are not in conflict. 
+In the case of transparency, one Member State (RO) aims to maintain transparency levels between 3 and 9 meters while the other (BG) aims for transparency to be comparable to waters not affected by anthropogenic pressure. Both Member States have also defined GES indicators relating to oxygen saturation of the upper water layer and both have also used the diatom dinoflaggelate ratio. One Member State (RO) has however also defined GES using macrophytes (Cystoseira, Zostera) while the other (BG) does not refer to macrophytobenthos. 
+The two Member States have linked their GES definition with the WFD normatives although for one Member State (RO), this seems to be limited to nutrient concentrations and coastal phytobenthos monitoring, dissolved oxygen status or other WFD normatives do not seem to be taken into account. No reference is made to the Black Sea Convention, which is explained by the fact that the BSC has not developed a regional approach to D5.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have provided an assessment of the pressure from eutrophication. The level of coherence of the assessment of the eutrophication pressure between the two Member States is considered as moderate to high. Both assessments focus on nutrients loads rather than levels in the environment or impacts. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both assessments are biased towards assessments of nutrient loads rather than levels of nutrients in their waters for which the information remains largely descriptive. Both countries cover nitrogen, phosphorous and organic matter in their assessments. In the reporting sheets, one Member State (RO) has reported urban and industrial sources as the main sources of nutrient input while the other (BG), in addition to these two sources, has added agriculture, forestry and shipping. Both countries also refer to rivers as nutrient sources affecting marine areas – Bulgaria refers to the Kamchiya River and Romania to the Danube and to a lesser extent to the Dniester.
+One of the Member States (RO) has also included transitional waters in their assessment, while the other has not. Both countries have covered impacts only to a very limited degree. One Member State (RO) has made judgements on the level of pressure but the other (BG) has not. Where trends in the level of pressure are described, they are indicated as declining. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have provided targets for Descriptor 5 but, as for the GES, the targets of one of the Member States (RO) seem to be proposed rather than adopted targets. One Member State (BG) has set 10 targets, which are all SMART. The other (RO) has set 8 targets that are specific but not all are measurable. The level of coherence in the setting of targets between the two Member States is moderate as a number of the targets deal with similar attributes but there is also a significant difference in the measurability of the targets. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The two Member States both have targets relating to chlorophyll-a levels, diatom dinoflagellate ratios, oxygen concentrations in the water column and reductions in nitrogen. Only one Member State (RO) has included a target relating to macrophytes, in line with the GES definition. 
+In its paper report, one Member State (RO) has defined a pressure-based target, which requires the reduction of nutrients from a number of different sources (e.g. phosphate-based detergents, farming, waste water treatment). However the target is not SMART as it does not include a threshold value or a quantitative trend. The other Member State’s targets (BG) are also structured such that once the relevant GES thresholds have been achieved, there is still an emphasis to continue pressure reduction (notably with regard to trend-based targets/indicators).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romania has not defined GES or set environmental targets for Descriptor 7, which means that it is not possible to compare the two Member States’ approaches and therefore not possible to make an assessment of coherence for GES and targets. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have reported very little on the pressure from hydrographical changes. The level of coherence of the initial assessments on the pressure from hydrographical changes between the two Member States is considered moderate to high. Both assessments are very limited and mainly focused on large-scale hydrographical changes. The assessments also indicate a lack of research data available in this area. Only one of the two Member States (BG) provides a judgement on the level of the pressure. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have reported very little on the pressure from hydrographical changes, one Member State (BG) in their reporting sheets states that there is no research evidence indicating significant alteration to the physical characteristics of the marine environment, the other (RO) mentions that changes to the thermal dynamic influence the plankton community. One Member State (BG) has judged the level of pressure for Descriptor 7 as acceptable (status is “good”); the other (RO) has not provided a judgement. Both countries seem to have focused their limited initial assessments on large-scale hydrographical changes. Only one of the Member States (RO) has reported on marine acidification but this is more related to fluctuations in pH due to biological phenomena than the long-term pH trend in the Black Sea.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Bulgaria and Romania have defined GES for Descriptor 8. Both countries have defined GES for the whole of their marine waters, not distinguishing between assessment areas. The level of coherence in the definitions of GES for D8 between the two Member States of the Black Sea is considered low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neither country has defined GES for criterion 8.2 of the Commission Decision on effects of contaminants, including acute pollution events (8.2.2). The two Member States justify the lack of definition for effects of contaminants by the lack of data and knowledge on indicators 8.2.1 (RO only) and 8.2.2 (RO and BG).
+The approaches used by the two countries differ quite significantly. First of all, one Member State (RO) has not really provided a definition of GES but rather an explanation of the standards it will use to measure if GES is achieved while the other Member State has provided a clear GES definition. Secondly, the standards used by the two countries differ. One Member State (RO) makes a clear reference to the Water Framework Directive (WFD), the Environmental Quality Standards (EQS) Directive and OSPAR’s Environmental Assessment Criteria (EAC), implying that concentrations of contaminants should remain within these regulatory levels. The other Member State (BG) requires concentration levels to be “close to the background levels”, with no further explanation of what is meant with “background levels”, and discharges from human activities “close to zero”. 
+One Member State (RO) has provided a detailed list of the substances covered by the GES definition, drawing on the list of priority substances from, inter alia, the WFD, OSPAR, HELCOM, MEDPOL and the BSC. The list includes both synthetic and non-synthetic substances (except mercury), to be measured in the three relevant matrices (water, biota and sediment). However, this Member State does not explain which substances should be measured in which matrix against which standard. The other Member State (BG) does not provide a list of the substances covered by the GES definition and since the definition does not refer to a specific regulation (e.g. the EQS), this cannot be inferred from context. It does not mention the three matrices for the measurement of contaminants.  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have undertaken an initial assessment on the level of pressure from contamination by synthetic and non-synthetic substances. There is a moderate level of coherence between the assessments of the pressure by contamination of the two Member States. Largely, the same contaminants have been assessed and the same main sources of contamination are identified by both countries. Neither Member State has provided an assessment of radionuclides and both Member States have presented very limited assessments for acute pollution. There are however some differences in the areas where the countries have reported or provided judgements. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have provided a quantitative assessment of the level of contamination. Both countries have reported the level of contamination from Pb, Cd, Ni and Cu. One Member State (BG) has also reported on Hg, Zn and Co and the other (RO) has also reported on Cr levels. In the reporting sheets, the input loads of heavy metals from land-based sources are provided for lead by one Member State (RO) and the aggregate amounts for a number of heavy metals (Cd, Zn, Pb, Cu, Ni) are provided by the other (BG). In addition, one Member State (RO) has reported on the input loads and sources of heavy metals in their paper report. Both countries have identified riverine inputs as the main source of heavy metals with those metals originating from industry and urban discharges. One Member State (BG) has also assessed the loads of heavy metals from air-based sources. Neither country presents relevant information on sea-based sources in the reporting sheets, both countries have however identified shipping as an important source of heavy metals and one (RO) has also identified also oil and gas. 
+In regard to environmental impacts, neither country has data to assess impacts although they provide concentration levels in certain species of shellfish and one (BG) also in specific fish species. 
+Both countries have also assessed synthetic compounds, both have provided data on the concentration levels of lindane, heptachlor, aldrin, dieldrin, endrin, DDT, DDD and DDE. One Member State (BG) has also assessed a number of PAHs (Benzo(a)pyrene, Benzo(a)anthracene, Benzo(b)fluoranthene, Benzo(k)fluoranthene, Benzo(g,h,i)perylene and Indeno(1,2,3-c,d)pyrene). The other Member State (RO) has assessed PAHs in general without naming the specific substances. One Member States (BG) has identified rivers as the main input source of synthetic contaminants Both Member States indicate industry, urban discharges and agriculture and forestry as the main sources of synthetic contaminants. Conclusions on the level of pollution are made by one Member State (RO) in relation to Directive 2008/105/EC (the EQS Directive) but not by the other (BG) due to a lack of sufficient data. Only one Member State (BG) has provided information on the level of pressure in functional groups which is all related to concentration levels in fish and shellfish. 
+One Member State (RO) assessed that 50-75% of its assessment area is affected by contamination by synthetic substances while the other does not provide such an assessment. 
+Acute pollution is covered briefly by both Member States focusing on hydrocarbon spills. One Member State (BG) reports that the level of pressure from acute pollution is acceptable (status is “good”) while the other (RO) does not provide a judgement. Neither Member State has provided an assessment of the pressure from radionuclides. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The two Member States have defined targets for Descriptor 8. One Member State (BG) has defined two targets and the other Member State (RO) has defined 10 targets in the reporting sheet and three in the paper report. Overall, the level of coherence in the setting of targets for D8 between the two Member States of the Black Sea is low. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The set of targets and associated indicators developed by the two countries are very different. One Member State (BG) has set two pressure targets, aiming to reduce input from sources of contamination, in particular atmospheric pollution and oil spills (despite the lack of GES indicator on acute pollution events). The associated indicators are actually indicators 8.1.1 and 8.2.2 of the Commission Decision. The other Member State (RO) has defined a number of state targets, which require concentration levels of certain contaminants, measured in various matrices, to be below regulatory levels. In the paper report, it has also defined a pressure target, requiring amount of contaminants in the marine environment to be low, with no threshold value or specification of the sources of contaminants targeted.  
+None of the two Member States has defined targets related to the biological effects of contaminants on ecosystem components, which is in line with the lack of provision on this issue in their GES definitions. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neither Bulgaria nor Romania has defined GES for Descriptor 9. One Member State (BG) does provide a reference to the relevant EU legislation for the monitoring of contaminants in seafood (Regulation 1881/2006) but does not clearly define what GES is in relation to D9 for its marine waters. The other Member States (RO) justifies the lack of GES definition by stating that there is not enough data to develop indicators for this descriptor. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only one Member State (BG) has made an assessment of contaminants in fish and seafood in relation to Regulation 1881/2006. The other Member State (RO) has not reported on contaminants in seafood. Overall, the level of coherence in low as only one country has provided quantified information. However both identify the same main sources of contamination and indicate that the situation is improving. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In relation to microbial pathogens, one Member State (BG) has made an assessment of the level of pressure and impacts while the other (RO) has only provided a general description on the issue of microbial pathogens in the black Sea. Both Member States identify urban wastewater and tourism as the main sources of this pressure. Both Member States also indicate that the situation is improving due to better waste water treatment. One Member State (BG) has provided a status assessment for bathing waters (31 out of 89 bathing water bodies are compliant).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only Bulgaria has defined environmental targets for Descriptor 9. It is therefore not possible to compare the two Member States’ approaches and therefore not possible to make an assessment of coherence. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neither Bulgaria nor Romania have defined GES or set environmental targets on Descriptor 10. In both cases, the justification provided is that there is not enough data and knowledge to develop GES indicators, as per the Commission Decision, and supporting environmental targets. 
+It is noteworthy that neither Bulgaria nor Romania have used the supporting documents on marine litter from UNEP (UNEP 2009: Marine Litter: a global Challenge) or the Black Sea Commission ((draft) Strategic Action Plan for Management and Abatement of marine litter in the Black Sea Region) to define what GES is in relation to marine litter in their marine waters.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have reported very little on the pressure from marine litter mainly identifying sources of litter and, in one case (BG), the main types of marine litter. The level of coherence of the initial assessments on the pressure from marine litter between the two Member States is considered high as both assessments are very limited, provide similar information and the same explanation for not providing status judgements on the pressure from marine litter. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Member States have identified shipping and fishing as sources while both also name other sources not identified by the other Member State. Neither Member State has assessed the level of pressure or impacts from marine litter or made a judgement in relation to GES. Both mention that it is due to a lack of appropriate assessment methodologies. 
+One Member State (BG) refers to the UNEP report on marine litter (UNEP 2009: Marine Litter: a global Challenge). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neither Bulgaria nor Romania have defined GES, carried out an initial assessment or set environmental targets for Descriptor 11. As for Descriptor 10, in both cases, the justification provided is that there is not enough data and knowledge to develop GES indicators, as per the Commission Decision, and supporting environmental targets. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conclusions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coverage of the MSFD articles (Art. 8, Art. 9 and Art. 10) for each of the 11 descriptors
+Coverage of the eleven descriptors for Descriptor 9 is not uniform. Three Member States (EE, LT, LV) have not defined GES for Descriptors 7, 10 and 11 and one of these Member States (LV) has also not defined GES for Descriptors 4 and 8. 
+A majority of Member States have made an initial assessment of all the relevant pressures, except two three Member States (LV, PL and SE), which did not make an assessment of the pressure from underwater noise and other forms of energy. One of these two three countries (LV) has also not reported on hydrographical processes and on marine litter.
+Four Member States out of seven eight did not define environmental targets for a number of descriptors: three Member States (DK, LT, LV) did not define targets for D7, three (LT, LV, SE) did not define targets for D11, two (LT, LV) did not define targets for D10 and one of these two also did not define targets for D4 and D8. 
+Descriptors 7, 10 and 11 are the descriptors for which there are most gaps. 
+Judgement on current status in relation to GES
+Only two three Member States (EE, LT, PL) have made systematic judgements on the current status of the marine environment (in relation to all relevant pressures/features), using indicators and criteria which are used both for Article 8 and for Article 9 (GES). One other Member State (DK) has made some firm statements on the current status in relation to GES but not systematically. 
+Use of EU requirements and standards
+All Member States but one (DK) have used EU requirements and standards in their definition of GES for the relevant descriptors (1, 3, 5, 7, 8 and 9). The remaining Member State (DK) has referred to the EU requirements and standards only in a limited manner. 
+Use of the Commission Decision criteria and indicators
+The approach adopted for the definition of GES varies substantially across the Member States of the Baltic region. Three Member States (EE, LT, LV) have defined GES only at indicator level, as a rule, but not systematically covering all indicators of the Commission Decision. One Two Member States (PL and SE) has defined GES at criteria and indicator level, closely following the structure of the Commission Decision. One Member State (FI) has defined GES at criteria level, as a rule. One Member State (DK) has defined GES only at descriptor level (with some exceptions for the biodiversity descriptors defined at criteria level). Finally, the remaining Member State (DE) has used a mixed approach, whereby it has defined GES at descriptor level for approximately half of the descriptors and at criteria/indicator level for the other half. 
+Certain criteria or indicators are almost never fully covered:
+- Only one Member State (DE) has included indicator 5.1.2 on nutrient ratios; only  threefour Member States (DE, EE, LV and PL) have covered indicators 5.2.3 on the abundance of opportunistic macroalgae and 5.2.4 on species shift in floristic composition in their GES definition of D5.
+- Criterion 9.1 on levels, number and frequency of contaminants is fully covered by only one Member State (SE). None of the other six Member States have defined GES for indicator 9.1.2 on the frequency of regulatory levels being exceeded.
+Reference to the work of the Regional Sea Conventions
+The work of HELCOM is extensively used and referred to by the Member States of the Baltic Sea marine region for almost all of the descriptors.
+A number of HELCOM documents are referred to in different places, including the HELCOM Baltic Sea Action Plan, the HELCOM HOLAS report and the HELCOM CORESET/TARGREV reports. In addition, specific tools/reports are used by the Member States for the individual descriptors:
+- Biodiversity: HELCOM list of species and habitats
+- NIS: HELCOM bio-pollution index; 
+- Commercial fisheries: HELCOM assessment of the status of the coastal fish community
+- Eutrophication: HELCOM HEAT; HELCOM assessments on eutrophication
+- Contaminants: HELCOM GES boundaries for priority hazardous substances; HELCOM assessments on hazardous substances
+- Marine litter: HELCOM Assessment of the marine litter problem
+Other regional sources of information have been used by some Member States, such as the Baltic Sea Alien Species Database for D2.
+Level of information on data/knowledge gaps and ways to address them
+A majorityHalf of Member States (DE, DK, LV , and SE) have systematically identified data and knowledge gaps, to varying levels of detail. Three of these Member States (DE, DK, SE) have also provided plans to close these gaps, mostly within the context of EU or Regional Seas Conventions work. Two Member States (FI, SE) have provided timelines regarding the development of GES and targets indicators for a number of descriptors where development is needed (in particular the biodiversity descriptor (D1) but also NIS (D2), commercial fish (D3), seafloor integrity (D6), hydrographical change (D7), marine litter (D10) and noise (D11)). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coverage of the MSFD articles (Art. 8, Art. 9 and Art. 10) for each of the 11 descriptors
+All Member States have defined GES for all descriptors.  
+A majority of Member States have made an initial assessment of all the relevant pressures, except two Member States (PT, SE), which did not make an assessment of the pressure from underwater noise and other forms of energy. 
+Four Member States out of ten did not define environmental targets for a number of descriptors: Two Member States (IE, PT) for the biodiversity descriptors (D1, 4 and 6); two (DK, PT) for Descriptor 7; two (IE, SE) for Descriptor 11 and one Member State (PT) for Descriptors 2 and 5.
+Judgement on current status in relation to GES
+Only a limited number of Member States in the region have made a judgement on the current status of the marine environment – in relation to certain pressures/features – using the same indicators and criteria for both Articles 8 and 9 (DK, ES, PT). The other Member States have either not made a conclusive judgement on the current status (e.g. FR) or have done so not in relation to GES but in relation to other standards (e.g. NL, BE).
+Use of EU requirements and standards
+Eight out of ten Member States have systematically used EU requirements and standards in their definition of GES for the relevant descriptors (1, 3, 5, 7, 8 and 9). The remaining two Member States (DK, PT) have referred to EU requirements and standards only in a very limited manner. 
+Use of the Commission Decision criteria and indicators
+Five Member States out of ten (BE, ES, FR, SE, UK) have defined their GES at least at criteria level as a rule (sometimes defining GES for one or two descriptors only at descriptor level). Two Member States (DE, IE) have used a mixed approach, whereby they have defined GES at descriptor level for approximately half of the descriptors and at criteria/indicator level for the other half. A final category of three Member States (DK, NL, PT) have defined GES only at descriptor level as a rule (with a few exceptions for one Member State (DK)). 
+Those Member States, which have defined GES at criteria level, have also used some of the Decision’s indicators. Only two Member States (FR, SE) have followed the structure of the Commission Decision quite consistently for all descriptors (but even these Member States have not defined GES for all individual indicators). Descriptor 10 is covered only at descriptor level by six Member States (DE, DK, ES, IE, NL, PT). 
+Certain criteria are almost never fully covered:
+- Only three Member States out of ten (ES, FR, SE) have covered criterion 2.2 on environmental impact of invasive NIS fully.
+- Only two Member States (DE, FR) have included indicator 5.1.2 on nutrient ratios and only four Member States have covered indicator 5.2.3 on the abundance of opportunistic macroalgae in their GES definition of D5.
+- Criterion 8.2 on effects of contaminants is fully covered by only two Member States (FR, SE). The other Member States have either not covered acute pollution events at all in their GES definition or they have covered it only through the inclusion of the OSPAR EcoQO on oiled guillemots, leaving out any mention of the occurrence, origin and extent of acute pollution events.
+- Criterion 9.1 on levels, number and frequency of contaminants is fully covered by only two Member States (FR, ES). None of the other eight Member States has defined GES for indicator 9.1.2 on the frequency of regulatory levels being exceeded.
+Reference to the work of the Regional Sea Conventions
+All Member States but one (PT) have regularly referred to, and used, the work of OSPAR in their GES definition, their initial assessment and the setting of their environmental targets. 
+Examples of the use of OSPAR’s advice and standards include:
+- For the biodiversity descriptors, OSPAR is referred to in the GES definition or in the targets (directly or in the accompanying text), by eight out of ten Member States (BE, DE, ES, FR, IE, NL, SE, UK). 
+- The OSPAR COMP procedure is used, or at least referred to, by six Member States out of ten (BE, DE, ES, FR, IE, UK) for the definition of GES for Descriptor 5. 
+- For Descriptor 7, the relevant OSPAR Advice is referred to, directly in the definition or in the accompanying text, only by four Member States (ES, FR, IE, NL). 
+- Six Member States out of ten (BE, DE, ES, FR, IE, UK) have used OSPAR’s Environmental Assessment Criteria (EAC) as reference levels for the concentration of hazardous substances in their definition of GES for Descriptor 8, in complement to (or instead of for one Member State (ES)) the Environmental Quality Standards (EQS). 
+- Five Member States (BE, DE, IE, NL, UK) have set a target which is either directly (using the same thresholds) or indirectly (using different thresholds or no threshold at all) related to the OSPAR EcoQO on northern fulmar. One Member State proposes to further research the usefulness of the EcoQO (DK) and one Member State has included it as an indicator in its GES definition (FR). The other three Member States (ES, PT, SE) have not used northern fulmars as indicators because the species is not present in their marine waters.
+All Member States refer to the 2010 OSPAR Quality Status Report (QSR) for their initial assessment, some (e.g. DE, SE, UK) more consistently than others (BE, DK, NL, PT). 
+Level of information on data/knowledge gaps and ways to address them
+All Member States but one (BE) have systematically identified data and knowledge gaps, to varying levels of detail. Out of these, five Member States have also, in general, provided plans to address these gaps (ES, FR, NL, SE, UK). Two Member States (DE, DK) rely mostly on on-going work at RSC or EU level to address data and knowledge gaps.  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLACK SEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The level of coherence was not assessed when the two Member States (or one of the two) did not report on an element (e.g. no GES or targets defined for D11). The assessment of coherence is based on the comparability of the elements reported by the two Member States. 
+Coverage of the MSFD articles (Art. 8, Art. 9 and Art. 10) for each of the 11 descriptors
+None of the Member States has defined GES for D9, D10 and D11. Consequently, the two countries have not set environmental targets for these descriptors (except D9 for which one Member State (BG) has set targets without having defined a GES). In addition, one of the Member State (RO) has not defined GES and targets for D7.
+Use of EU requirements and standards
+Both Member States have used EU requirements and standards where relevant (i.e. D1, D3, D5, D8) but neither necessarily systematically. 
+Use of the Commission Decision criteria and indicators
+One Member State (RO) has defined GES as a rule at indicator level but not always following the structure of the Commission Decision or using the same indicators. The other Member State has used a mixed approach, defining GES at descriptor, criteria or indicator level, depending on the descriptor. 
+The Commission Decision indicators have been used by both countries to specify some of their targets (e.g. for D8), either using them literally (BG) or specifying them further (RO). 
+Reference to the work of the Regional Sea Conventions
+The two Member States have made very limited references to the work of the Bucharest Convention when defining their GES, carrying out their initial assessment or setting their targets. The only references to the Bucharest Convention relates to its list of protected species and its list of priority hazardous substances.  
+Level of information on data/knowledge gaps and ways to address them
+One Member State (BG) has identified data and knowledge gaps much more consistently and systematically than the other (RO). This Member State has also provided a number of high-level recommendations / plans to address these gaps for descriptors for which knowledge gaps are very important (e.g. D10, D11). But timeline and concrete steps to be taken to address the gaps are not provided. 
+Coverage of the MSFD articles (Art. 8, Art. 9 and Art. 10) for each of the 11 descriptors
+None of the Member States has defined GES for D9, D10 and D11. Consequently, the two countries have not set environmental targets for these descriptors (except D9 for which one Member State (BG) has set targets without having defined a GES). In addition, one of the Member State (RO) has not defined GES and targets for D7.
+Use of EU requirements and standards
+Both Member States have used EU requirements and standards where relevant (i.e. D1, D3, D5, D8) but neither necessarily systematically. 
+Use of the Commission Decision criteria and indicators
+One Member State (RO) has defined GES as a rule at indicator level but not always following the structure of the Commission Decision or using the same indicators. The other Member State has used a mixed approach, defining GES at descriptor, criteria or indicator level, depending on the descriptor. 
+The Commission Decision indicators have been used by both countries to specify some of their targets (e.g. for D8), either using them literally (BG) or specifying them further (RO). 
+Reference to the work of the Regional Sea Conventions
+The two Member States have made very limited references to the work of the Bucharest Convention when defining their GES, carrying out their initial assessment or setting their targets. The only references to the Bucharest Convention relates to its list of protected species and its list of priority hazardous substances.  
+Level of information on data/knowledge gaps and ways to address them
+One Member State (BG) has identified data and knowledge gaps much more consistently and systematically than the other (RO). This Member State has also provided a number of high-level recommendations / plans to address these gaps for descriptors for which knowledge gaps are very important (e.g. D10, D11). But timeline and concrete steps to be taken to address the gaps are not provided. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coverage of the MSFD articles (Art. 8, Art. 9 and Art. 10) for each of the 11 descriptors
+All Member States have defined GES for all descriptors, except one two Member States (CY, MT) which haves not defined GES for Descriptor 4. 
+A majority of Member States have made an initial assessment of all the relevant pressures, except two Member States (CY, IT), which did not make an assessment of the pressure from underwater noise and other forms of energy and one Member State (IT), which did not make an assessment of the contamination of fish and seafood by hazardous substances. 
+Four Five Member States out of six seven did not define environmental targets for a number of descriptors: one two Member States (CY, MT) did not define targets for D2 and D4, another (FR) did not define targets for D5, three Member States (CY, FR, IT) did not define targets for D7, two three (FR, IT, MT) did not define targets for D9 and three (CY, EL, IT) did not define targets for D11.
+Judgement on current status in relation to GES
+Many Member States in the region have attempted to make a judgement on the current status of their marine environment – in relation to certain pressures/features – using indicators and criteria which are used both for Article 8 and for Article 9 (GES). However, most of the time the indicators and criteria are not quantitative and/or are based on expert judgement. 
+Use of EU requirements and standards
+Four out of six seven Member States (ES, FR, IT, SI) have systematically used EU requirements and standards in their definition of GES for the relevant descriptors (1, 3, 5, 7, 8 and 9). The remaining two three Member States have referred to the EU requirements and standards only in a very limited manner (CY, EL, MT). 
+Use of the Commission Decision criteria and indicators
+As a rule, all Member States in the marine region but one (CY) have defined GES at least at criteria level, using some or all of the criteria of the Commission Decision for each Descriptor. One Member State (CY) has defined GES as a rule at descriptor level. Most Member States have also used some of the Decision’s indicators. Only one Member State (FR) has followed the structure of the Commission Decision quite consistently for all descriptors. 
+Descriptors 7, 10 and 11 are often covered only at descriptor level, respectively by three four (CY, ES, MT, SI), four five (CY, EL, ES, MT, SI) and three four (CY, ES, MT, IT) Member States. 
+Certain criteria are almost never fully covered:
+- Criterion 2.2 on environmental impact of invasive NIS is never fully covered by the Member States. Two Three Member States (CY, EL, MT) have not defined GES for criterion 2.2 at all, three Member States (FR, IT, SI) have not defined GES for indicator 2.2.1 on the ratio between invasive NIS and native species and one Member State (ES) has not defined GES for indicator 2.2.2 on the impacts of NIS.
+- Only two three Member States (FR, IT, MT) have included indicator 5.1.2 on nutrient ratios in their GES definition for D5.
+- Criterion 8.2 on effects of contaminants is fully covered by only one Member State (FR). None of the other fiveFive Member States (CY, EL, ES, IT, SI) have nots defined GES for indicator 8.2.2 on acute pollution events and one Member State (MT) has not defined GES for indicator 8.2.1 on biological effects.
+- Criterion 9.1 on levels, number and frequency of contaminants is fully covered by only two Member States (FR, ES). None of the other four five Member States has defined GES for indicator 9.1.2 on the frequency of regulatory levels being exceeded.
+Reference to the work of the Regional Sea Conventions
+Only half of the countries have regularly referred to the work of the Barcelona Convention in their initial assessment (CY, ES, FR, MT). However, there is very rarely a specific reference to the Barcelona Convention Ecosystem Approach (e.g. France in its introduction to GES mentions that it is taken into account in the design of indicators and criteriaFR, MT). The Barcelona list of protected species is mentioned by four Member States (CY, ES, FR, IT). 
+Most Member States have also made references to, and/or used, OSPAR standards. In particular, OSPAR’s Environmental Assessment Criteria have been used by four Member States (EL, ES, FR, SI) in their definition of GES for D8.
+Level of information on data/knowledge gaps and ways to address them
+A majority of Member States (EL, ES, FR, IT, MT, SI) have systematically identified data and knowledge gaps, to varying levels of detail. All of these Member States but one two (EL, MT) have also provided plans to close these gaps. In a number of cases (ES, IT, SI) the plans to address the gaps are integrated in the form of high-level objectives/targets focused on further research and improved monitoring. 
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Field name</t>
   </si>
   <si>
@@ -538,9 +1494,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -674,7 +1630,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -683,6 +1639,26 @@
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -720,7 +1696,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
     <fill>
@@ -736,7 +1712,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -757,6 +1733,13 @@
       <bottom style="thin">
         <color rgb="FF808080"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -836,7 +1819,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -873,12 +1856,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -911,13 +1922,13 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF996600"/>
@@ -971,29 +1982,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K145"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K38" activeCellId="0" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="157.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="48.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="157.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.42"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1311,7 +2322,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="242.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="191.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>11</v>
       </c>
@@ -1346,7 +2357,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="269.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>11</v>
       </c>
@@ -1486,7 +2497,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="140.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>11</v>
       </c>
@@ -1521,7 +2532,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="178.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>11</v>
       </c>
@@ -1661,7 +2672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>11</v>
       </c>
@@ -1731,7 +2742,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="165.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>11</v>
       </c>
@@ -1766,7 +2777,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>11</v>
       </c>
@@ -1801,7 +2812,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="178.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>11</v>
       </c>
@@ -1836,7 +2847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>11</v>
       </c>
@@ -2081,7 +3092,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="140.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>11</v>
       </c>
@@ -2116,7 +3127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="140.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>11</v>
       </c>
@@ -2151,7 +3162,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>11</v>
       </c>
@@ -2221,7 +3232,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="357" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="165.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>11</v>
       </c>
@@ -2256,7 +3267,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="78.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>11</v>
       </c>
@@ -2291,59 +3302,3065 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="8"/>
+    <row r="38" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="8" t="n">
+        <v>41822</v>
+      </c>
       <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="8"/>
+      <c r="H38" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J38" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="191.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="8" t="n">
+        <v>41677</v>
+      </c>
       <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F40" s="4"/>
-      <c r="I40" s="10"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F41" s="4"/>
-      <c r="J41" s="1"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F42" s="4"/>
-      <c r="I42" s="10"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F43" s="4"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F44" s="4"/>
-      <c r="I44" s="10"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F45" s="4"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F46" s="4"/>
-      <c r="I46" s="10"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F47" s="4"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F48" s="4"/>
+      <c r="H39" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J39" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="J40" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G41" s="7"/>
+      <c r="H41" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="J41" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="360" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J42" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="165.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G43" s="7"/>
+      <c r="H43" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="J43" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J44" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G45" s="7"/>
+      <c r="H45" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="J45" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="375" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="J46" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K46" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="165.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G47" s="7"/>
+      <c r="H47" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="J47" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K47" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G48" s="7"/>
+      <c r="H48" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J48" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K48" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G49" s="7"/>
+      <c r="H49" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="J49" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K49" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="140.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G50" s="7"/>
+      <c r="H50" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="J50" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G51" s="7"/>
+      <c r="H51" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I51" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="J51" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K51" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="216.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G52" s="7"/>
+      <c r="H52" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="J52" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K52" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="395.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G53" s="7"/>
+      <c r="H53" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="J53" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G54" s="7"/>
+      <c r="H54" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="J54" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="267.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G55" s="7"/>
+      <c r="H55" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="J55" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K55" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="280.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G56" s="7"/>
+      <c r="H56" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="J56" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K56" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="318.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G57" s="7"/>
+      <c r="H57" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="J57" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K57" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G58" s="7"/>
+      <c r="H58" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="J58" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K58" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="216.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F59" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G59" s="7"/>
+      <c r="H59" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="I59" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="J59" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K59" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="140.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G60" s="7"/>
+      <c r="H60" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="J60" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K60" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G61" s="7"/>
+      <c r="H61" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="J61" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K61" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="267.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="7"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="J62" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K62" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="306" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="J63" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K63" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="216.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D64" s="7"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="J64" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="165.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G65" s="7"/>
+      <c r="H65" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="J65" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K65" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" s="8" t="n">
+        <v>41677</v>
+      </c>
+      <c r="G66" s="7"/>
+      <c r="H66" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="J66" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K66" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="267.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" s="8" t="n">
+        <v>41691</v>
+      </c>
+      <c r="G67" s="7"/>
+      <c r="H67" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="J67" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K67" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" s="8" t="n">
+        <v>41692</v>
+      </c>
+      <c r="G68" s="7"/>
+      <c r="H68" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="J68" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K68" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="216.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" s="8" t="n">
+        <v>41693</v>
+      </c>
+      <c r="G69" s="7"/>
+      <c r="H69" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="I69" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="J69" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K69" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="280.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F70" s="8" t="n">
+        <v>41695</v>
+      </c>
+      <c r="G70" s="7"/>
+      <c r="H70" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="I70" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="J70" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K70" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71" s="8" t="n">
+        <v>41696</v>
+      </c>
+      <c r="G71" s="7"/>
+      <c r="H71" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="J71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K71" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F72" s="8" t="n">
+        <v>41697</v>
+      </c>
+      <c r="G72" s="7"/>
+      <c r="H72" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="J72" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K72" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F73" s="8" t="n">
+        <v>41699</v>
+      </c>
+      <c r="G73" s="7"/>
+      <c r="H73" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="I73" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="J73" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K73" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="I74" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="J74" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K74" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J75" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K75" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="I76" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="J76" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K76" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="I77" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="J77" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K77" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="255" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="I78" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="J78" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K78" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="I79" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J79" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K79" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="I80" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="J80" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K80" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="I81" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="J81" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K81" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="280.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="I82" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="J82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K82" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="I83" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J83" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K83" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="I84" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="J84" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K84" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="I85" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="J85" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K85" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H86" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J86" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K86" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H87" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J87" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K87" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H88" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J88" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K88" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="191.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H89" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J89" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K89" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H90" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="J90" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K90" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H91" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J91" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K91" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H92" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="J92" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K92" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="293.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H93" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="J93" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K93" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H94" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J94" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K94" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="178.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J95" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K95" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H96" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J96" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K96" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H97" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J97" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K97" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="369.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H98" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J98" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K98" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="255" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H99" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J99" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K99" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="255" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H100" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J100" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K100" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H101" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J101" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K101" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="229.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H102" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J102" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K102" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H103" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J103" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K103" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H104" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J104" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K104" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H105" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J105" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K105" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="165.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H106" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J106" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K106" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H107" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J107" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K107" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H108" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J108" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K108" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H109" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J109" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K109" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="344.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J110" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K110" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H111" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J111" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K111" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="369.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C112" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J112" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K112" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="165.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H113" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="J113" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K113" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="344.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D114" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J114" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K114" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D115" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H115" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J115" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K115" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="369.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D116" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J116" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K116" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="165.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H117" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="J117" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K117" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="344.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J118" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K118" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D119" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H119" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J119" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K119" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="369.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J120" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K120" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="165.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H121" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="J121" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K121" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D122" s="7"/>
+      <c r="H122" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="J122" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K122" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D123" s="7"/>
+      <c r="H123" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="J123" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K123" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="53.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D124" s="7"/>
+      <c r="H124" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="J124" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K124" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H125" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J125" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K125" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D126" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H126" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J126" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K126" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D127" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H127" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J127" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K127" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D128" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H128" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="J128" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K128" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H129" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="J129" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K129" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="140.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D130" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H130" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="J130" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K130" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="56.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D131" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H131" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="J131" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D132" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H132" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J132" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K132" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D133" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H133" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="I133" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="J133" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="191.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D134" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H134" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="I134" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J134" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K134" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="293.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D135" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H135" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="I135" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J135" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K135" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D136" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H136" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="I136" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="J136" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K136" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D137" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H137" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="I137" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J137" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D138" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H138" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="I138" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J138" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K138" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D139" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H139" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="I139" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="J139" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="168.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D140" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="I140" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="J140" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K140" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D141" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H141" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="I141" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="J141" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="168.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C142" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D142" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="I142" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="J142" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K142" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="78.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H143" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="J143" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K143" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="78.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H144" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="I144" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="J144" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K144" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H145" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="I145" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="J145" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K145" s="0" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2367,7 +6384,76 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="127.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="14" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2377,22 +6463,22 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>103</v>
+        <v>282</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>283</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>105</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,7 +6486,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>106</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2408,7 +6494,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>107</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2416,7 +6502,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>108</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2424,7 +6510,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>109</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,7 +6518,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>110</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2440,7 +6526,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>111</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2448,7 +6534,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>112</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2456,7 +6542,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>113</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2464,7 +6550,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>113</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2472,7 +6558,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>114</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2480,7 +6566,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>115</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>